<commit_message>
v0.0.7 - write the {ungroup} processes for the COD data. Change COD selection by eliminating some cancers and adding the maternal mortality.
</commit_message>
<xml_diff>
--- a/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
+++ b/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpascariu\Documents\R-Repos\MortalityCauses\data-raw\GBD_2019_Data_Tools_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5789E9E8-2A7C-466A-9DE5-48047752BF32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E960DA34-BC28-4EB8-BC97-1CBDFF2430F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52400,7 +52400,7 @@
   <dimension ref="A1:K361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -54572,7 +54572,7 @@
         <v>72</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>1607</v>
+        <v>828</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>1612</v>
@@ -55927,7 +55927,7 @@
         <v>118</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>920</v>
+        <v>962</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>876</v>
@@ -56043,7 +56043,7 @@
         <v>122</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>928</v>
+        <v>962</v>
       </c>
       <c r="K123" s="1" t="s">
         <v>876</v>

</xml_diff>

<commit_message>
v0.0.8 - Correct COD percentage calculation. We want the distribution of the COD within each age group. NOT the distribution of the age-groups within each COD.
</commit_message>
<xml_diff>
--- a/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
+++ b/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpascariu\Documents\R-Repos\MortalityCauses\data-raw\GBD_2019_Data_Tools_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E960DA34-BC28-4EB8-BC97-1CBDFF2430F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0A2F04-1C00-444E-87D0-B41FDDDB9215}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4852,9 +4852,6 @@
     <t>app_selection</t>
   </si>
   <si>
-    <t>Other Communicable Diseases: maternal, neonatal, and nutritional</t>
-  </si>
-  <si>
     <t>Other Non-Communicable Diseases</t>
   </si>
   <si>
@@ -4874,6 +4871,10 @@
   </si>
   <si>
     <t>Injuries: Transport and Unintentional</t>
+  </si>
+  <si>
+    <t>Other Communicable Diseases: 
+infections and nutritional deficiencies</t>
   </si>
 </sst>
 </file>
@@ -5381,12 +5382,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -52399,9 +52403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K361"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52451,7 +52455,7 @@
         <v>1606</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -52477,10 +52481,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -52506,10 +52510,10 @@
         <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -52538,7 +52542,7 @@
         <v>689</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -52564,10 +52568,10 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -52593,10 +52597,10 @@
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -52622,10 +52626,10 @@
         <v>6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -52651,10 +52655,10 @@
         <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -52680,10 +52684,10 @@
         <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -52709,10 +52713,10 @@
         <v>9</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -52738,10 +52742,10 @@
         <v>10</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -52767,10 +52771,10 @@
         <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -52796,10 +52800,10 @@
         <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -52828,10 +52832,10 @@
         <v>711</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -52860,10 +52864,10 @@
         <v>711</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -52889,10 +52893,10 @@
         <v>15</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -52921,7 +52925,7 @@
         <v>716</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -52947,10 +52951,10 @@
         <v>17</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -52979,10 +52983,10 @@
         <v>711</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -53008,10 +53012,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -53037,10 +53041,10 @@
         <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -53066,10 +53070,10 @@
         <v>21</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -53095,10 +53099,10 @@
         <v>22</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -53124,10 +53128,10 @@
         <v>23</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -53153,13 +53157,13 @@
         <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>957</v>
       </c>
@@ -53181,11 +53185,11 @@
       <c r="G26">
         <v>25</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>1607</v>
+      <c r="J26" s="5" t="s">
+        <v>1614</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -53211,10 +53215,10 @@
         <v>26</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -53240,10 +53244,10 @@
         <v>27</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -53269,10 +53273,10 @@
         <v>28</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -53298,10 +53302,10 @@
         <v>29</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -53327,10 +53331,10 @@
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -53356,13 +53360,13 @@
         <v>31</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>344</v>
       </c>
@@ -53384,11 +53388,11 @@
       <c r="G33">
         <v>32</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>1607</v>
+      <c r="J33" s="5" t="s">
+        <v>1614</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -53414,10 +53418,10 @@
         <v>33</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -53443,10 +53447,10 @@
         <v>34</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -53472,10 +53476,10 @@
         <v>35</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -53501,10 +53505,10 @@
         <v>36</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -53533,10 +53537,10 @@
         <v>711</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -53562,10 +53566,10 @@
         <v>38</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -53591,10 +53595,10 @@
         <v>39</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -53620,10 +53624,10 @@
         <v>40</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -53649,10 +53653,10 @@
         <v>41</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -53681,10 +53685,10 @@
         <v>711</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -53713,10 +53717,10 @@
         <v>711</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -53745,10 +53749,10 @@
         <v>711</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -53774,10 +53778,10 @@
         <v>45</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -53803,10 +53807,10 @@
         <v>46</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -53832,10 +53836,10 @@
         <v>47</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -53861,10 +53865,10 @@
         <v>48</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -53890,10 +53894,10 @@
         <v>49</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -53922,10 +53926,10 @@
         <v>711</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -53954,10 +53958,10 @@
         <v>711</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -53986,10 +53990,10 @@
         <v>711</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -54018,10 +54022,10 @@
         <v>711</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -54047,10 +54051,10 @@
         <v>54</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -54076,10 +54080,10 @@
         <v>55</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -54108,10 +54112,10 @@
         <v>711</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -54137,13 +54141,13 @@
         <v>57</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>961</v>
       </c>
@@ -54165,11 +54169,11 @@
       <c r="G59">
         <v>58</v>
       </c>
-      <c r="J59" s="4" t="s">
-        <v>1607</v>
+      <c r="J59" s="5" t="s">
+        <v>1614</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -54195,10 +54199,10 @@
         <v>59</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -54224,10 +54228,10 @@
         <v>60</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -54253,10 +54257,10 @@
         <v>61</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -54282,10 +54286,10 @@
         <v>62</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -54311,10 +54315,10 @@
         <v>63</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -54340,10 +54344,10 @@
         <v>64</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -54369,10 +54373,10 @@
         <v>65</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -54398,10 +54402,10 @@
         <v>66</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -54427,10 +54431,10 @@
         <v>67</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -54456,10 +54460,10 @@
         <v>68</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -54485,10 +54489,10 @@
         <v>69</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -54514,10 +54518,10 @@
         <v>70</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -54543,10 +54547,10 @@
         <v>71</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -54575,7 +54579,7 @@
         <v>828</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -54601,10 +54605,10 @@
         <v>73</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -54630,10 +54634,10 @@
         <v>74</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -54659,10 +54663,10 @@
         <v>75</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -54688,10 +54692,10 @@
         <v>76</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -54717,10 +54721,10 @@
         <v>77</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -54746,10 +54750,10 @@
         <v>78</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -54775,10 +54779,10 @@
         <v>79</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -54807,10 +54811,10 @@
         <v>711</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -54839,10 +54843,10 @@
         <v>711</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -54871,10 +54875,10 @@
         <v>711</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -54900,10 +54904,10 @@
         <v>83</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -54929,10 +54933,10 @@
         <v>84</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -54958,10 +54962,10 @@
         <v>85</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -54987,10 +54991,10 @@
         <v>86</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -55016,10 +55020,10 @@
         <v>87</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -55045,10 +55049,10 @@
         <v>88</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -55074,13 +55078,13 @@
         <v>89</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>386</v>
       </c>
@@ -55102,11 +55106,11 @@
       <c r="G91">
         <v>90</v>
       </c>
-      <c r="J91" s="4" t="s">
-        <v>1607</v>
+      <c r="J91" s="5" t="s">
+        <v>1614</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -55132,10 +55136,10 @@
         <v>91</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -55164,10 +55168,10 @@
         <v>711</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -55196,10 +55200,10 @@
         <v>711</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -55228,10 +55232,10 @@
         <v>711</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -55257,10 +55261,10 @@
         <v>95</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -55286,7 +55290,7 @@
         <v>96</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>876</v>
@@ -55315,7 +55319,7 @@
         <v>97</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>876</v>
@@ -55547,7 +55551,7 @@
         <v>105</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>876</v>
@@ -55576,7 +55580,7 @@
         <v>106</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>876</v>
@@ -55605,7 +55609,7 @@
         <v>107</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>876</v>
@@ -55634,7 +55638,7 @@
         <v>108</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>876</v>
@@ -55663,7 +55667,7 @@
         <v>109</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>876</v>
@@ -55779,7 +55783,7 @@
         <v>113</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>876</v>
@@ -55866,7 +55870,7 @@
         <v>116</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>876</v>
@@ -55898,7 +55902,7 @@
         <v>711</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>876</v>
@@ -56362,7 +56366,7 @@
         <v>133</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>876</v>
@@ -56391,7 +56395,7 @@
         <v>134</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K135" s="1" t="s">
         <v>876</v>
@@ -56420,7 +56424,7 @@
         <v>135</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K136" s="1" t="s">
         <v>876</v>
@@ -56449,7 +56453,7 @@
         <v>136</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K137" s="1" t="s">
         <v>876</v>
@@ -56478,7 +56482,7 @@
         <v>137</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>876</v>
@@ -56565,7 +56569,7 @@
         <v>140</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K141" s="1" t="s">
         <v>876</v>
@@ -56597,7 +56601,7 @@
         <v>711</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K142" s="1" t="s">
         <v>876</v>
@@ -56629,7 +56633,7 @@
         <v>711</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K143" s="1" t="s">
         <v>876</v>
@@ -56661,7 +56665,7 @@
         <v>711</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K144" s="1" t="s">
         <v>876</v>
@@ -56690,7 +56694,7 @@
         <v>144</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K145" s="1" t="s">
         <v>876</v>
@@ -56806,7 +56810,7 @@
         <v>148</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>876</v>
@@ -56835,7 +56839,7 @@
         <v>149</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>876</v>
@@ -56864,7 +56868,7 @@
         <v>150</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K151" s="1" t="s">
         <v>876</v>
@@ -56951,7 +56955,7 @@
         <v>153</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>876</v>
@@ -56980,7 +56984,7 @@
         <v>154</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K155" s="1" t="s">
         <v>876</v>
@@ -57009,7 +57013,7 @@
         <v>155</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>876</v>
@@ -57067,7 +57071,7 @@
         <v>157</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>876</v>
@@ -57096,7 +57100,7 @@
         <v>158</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K159" s="1" t="s">
         <v>876</v>
@@ -57125,7 +57129,7 @@
         <v>159</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>876</v>
@@ -57331,7 +57335,7 @@
         <v>166</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K167" s="1" t="s">
         <v>876</v>
@@ -57360,7 +57364,7 @@
         <v>167</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K168" s="1" t="s">
         <v>876</v>
@@ -57389,7 +57393,7 @@
         <v>168</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K169" s="1" t="s">
         <v>876</v>
@@ -57418,7 +57422,7 @@
         <v>169</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K170" s="1" t="s">
         <v>876</v>
@@ -57447,7 +57451,7 @@
         <v>170</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K171" s="1" t="s">
         <v>876</v>
@@ -57476,7 +57480,7 @@
         <v>171</v>
       </c>
       <c r="J172" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K172" s="1" t="s">
         <v>876</v>
@@ -57505,7 +57509,7 @@
         <v>172</v>
       </c>
       <c r="J173" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K173" s="1" t="s">
         <v>876</v>
@@ -57534,7 +57538,7 @@
         <v>173</v>
       </c>
       <c r="J174" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K174" s="1" t="s">
         <v>876</v>
@@ -57563,7 +57567,7 @@
         <v>174</v>
       </c>
       <c r="J175" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K175" s="1" t="s">
         <v>876</v>
@@ -57621,7 +57625,7 @@
         <v>176</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K177" s="1" t="s">
         <v>876</v>
@@ -57650,7 +57654,7 @@
         <v>177</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K178" s="1" t="s">
         <v>876</v>
@@ -57679,7 +57683,7 @@
         <v>178</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K179" s="1" t="s">
         <v>876</v>
@@ -57708,7 +57712,7 @@
         <v>179</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K180" s="1" t="s">
         <v>876</v>
@@ -57737,7 +57741,7 @@
         <v>180</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K181" s="1" t="s">
         <v>876</v>
@@ -57766,7 +57770,7 @@
         <v>181</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K182" s="1" t="s">
         <v>876</v>
@@ -57795,7 +57799,7 @@
         <v>182</v>
       </c>
       <c r="J183" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K183" s="1" t="s">
         <v>876</v>
@@ -57824,7 +57828,7 @@
         <v>183</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K184" s="1" t="s">
         <v>876</v>
@@ -57853,7 +57857,7 @@
         <v>184</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K185" s="1" t="s">
         <v>876</v>
@@ -57885,7 +57889,7 @@
         <v>711</v>
       </c>
       <c r="J186" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K186" s="1" t="s">
         <v>876</v>
@@ -57914,7 +57918,7 @@
         <v>186</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K187" s="1" t="s">
         <v>876</v>
@@ -57943,7 +57947,7 @@
         <v>187</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K188" s="1" t="s">
         <v>876</v>
@@ -57972,7 +57976,7 @@
         <v>188</v>
       </c>
       <c r="J189" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K189" s="1" t="s">
         <v>876</v>
@@ -58001,7 +58005,7 @@
         <v>189</v>
       </c>
       <c r="J190" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K190" s="1" t="s">
         <v>876</v>
@@ -58030,7 +58034,7 @@
         <v>190</v>
       </c>
       <c r="J191" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K191" s="1" t="s">
         <v>876</v>
@@ -58059,7 +58063,7 @@
         <v>191</v>
       </c>
       <c r="J192" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K192" s="1" t="s">
         <v>876</v>
@@ -58088,7 +58092,7 @@
         <v>192</v>
       </c>
       <c r="J193" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K193" s="1" t="s">
         <v>876</v>
@@ -58117,7 +58121,7 @@
         <v>193</v>
       </c>
       <c r="J194" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K194" s="1" t="s">
         <v>876</v>
@@ -58175,7 +58179,7 @@
         <v>195</v>
       </c>
       <c r="J196" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K196" s="1" t="s">
         <v>876</v>
@@ -58204,7 +58208,7 @@
         <v>196</v>
       </c>
       <c r="J197" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K197" s="1" t="s">
         <v>876</v>
@@ -58233,7 +58237,7 @@
         <v>197</v>
       </c>
       <c r="J198" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K198" s="1" t="s">
         <v>876</v>
@@ -58262,7 +58266,7 @@
         <v>198</v>
       </c>
       <c r="J199" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K199" s="1" t="s">
         <v>876</v>
@@ -58291,7 +58295,7 @@
         <v>199</v>
       </c>
       <c r="J200" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K200" s="1" t="s">
         <v>876</v>
@@ -58323,7 +58327,7 @@
         <v>711</v>
       </c>
       <c r="J201" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K201" s="1" t="s">
         <v>876</v>
@@ -58355,7 +58359,7 @@
         <v>711</v>
       </c>
       <c r="J202" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K202" s="1" t="s">
         <v>876</v>
@@ -58387,7 +58391,7 @@
         <v>711</v>
       </c>
       <c r="J203" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K203" s="1" t="s">
         <v>876</v>
@@ -58416,7 +58420,7 @@
         <v>203</v>
       </c>
       <c r="J204" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K204" s="1" t="s">
         <v>876</v>
@@ -58445,7 +58449,7 @@
         <v>204</v>
       </c>
       <c r="J205" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K205" s="1" t="s">
         <v>876</v>
@@ -58477,7 +58481,7 @@
         <v>711</v>
       </c>
       <c r="J206" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K206" s="1" t="s">
         <v>876</v>
@@ -58509,7 +58513,7 @@
         <v>711</v>
       </c>
       <c r="J207" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K207" s="1" t="s">
         <v>876</v>
@@ -58541,7 +58545,7 @@
         <v>711</v>
       </c>
       <c r="J208" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K208" s="1" t="s">
         <v>876</v>
@@ -58573,7 +58577,7 @@
         <v>711</v>
       </c>
       <c r="J209" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K209" s="1" t="s">
         <v>876</v>
@@ -58605,7 +58609,7 @@
         <v>711</v>
       </c>
       <c r="J210" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K210" s="1" t="s">
         <v>876</v>
@@ -58637,7 +58641,7 @@
         <v>711</v>
       </c>
       <c r="J211" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K211" s="1" t="s">
         <v>876</v>
@@ -58666,7 +58670,7 @@
         <v>211</v>
       </c>
       <c r="J212" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K212" s="1" t="s">
         <v>876</v>
@@ -58695,7 +58699,7 @@
         <v>212</v>
       </c>
       <c r="J213" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K213" s="1" t="s">
         <v>876</v>
@@ -58724,7 +58728,7 @@
         <v>213</v>
       </c>
       <c r="J214" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K214" s="1" t="s">
         <v>876</v>
@@ -58756,7 +58760,7 @@
         <v>711</v>
       </c>
       <c r="J215" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K215" s="1" t="s">
         <v>876</v>
@@ -58788,7 +58792,7 @@
         <v>711</v>
       </c>
       <c r="J216" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K216" s="1" t="s">
         <v>876</v>
@@ -58820,7 +58824,7 @@
         <v>711</v>
       </c>
       <c r="J217" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K217" s="1" t="s">
         <v>876</v>
@@ -58852,7 +58856,7 @@
         <v>711</v>
       </c>
       <c r="J218" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K218" s="1" t="s">
         <v>876</v>
@@ -58884,7 +58888,7 @@
         <v>711</v>
       </c>
       <c r="J219" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K219" s="1" t="s">
         <v>876</v>
@@ -58913,7 +58917,7 @@
         <v>219</v>
       </c>
       <c r="J220" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K220" s="1" t="s">
         <v>876</v>
@@ -58942,7 +58946,7 @@
         <v>220</v>
       </c>
       <c r="J221" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K221" s="1" t="s">
         <v>876</v>
@@ -58971,7 +58975,7 @@
         <v>221</v>
       </c>
       <c r="J222" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K222" s="1" t="s">
         <v>876</v>
@@ -59000,7 +59004,7 @@
         <v>222</v>
       </c>
       <c r="J223" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K223" s="1" t="s">
         <v>876</v>
@@ -59029,7 +59033,7 @@
         <v>223</v>
       </c>
       <c r="J224" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K224" s="1" t="s">
         <v>876</v>
@@ -59058,7 +59062,7 @@
         <v>224</v>
       </c>
       <c r="J225" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K225" s="1" t="s">
         <v>876</v>
@@ -59090,7 +59094,7 @@
         <v>711</v>
       </c>
       <c r="J226" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K226" s="1" t="s">
         <v>876</v>
@@ -59119,7 +59123,7 @@
         <v>226</v>
       </c>
       <c r="J227" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K227" s="1" t="s">
         <v>876</v>
@@ -59177,7 +59181,7 @@
         <v>228</v>
       </c>
       <c r="J229" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K229" s="1" t="s">
         <v>876</v>
@@ -59206,7 +59210,7 @@
         <v>229</v>
       </c>
       <c r="J230" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K230" s="1" t="s">
         <v>876</v>
@@ -59235,7 +59239,7 @@
         <v>230</v>
       </c>
       <c r="J231" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K231" s="1" t="s">
         <v>876</v>
@@ -59264,7 +59268,7 @@
         <v>231</v>
       </c>
       <c r="J232" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K232" s="1" t="s">
         <v>876</v>
@@ -59293,7 +59297,7 @@
         <v>232</v>
       </c>
       <c r="J233" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K233" s="1" t="s">
         <v>876</v>
@@ -59322,7 +59326,7 @@
         <v>233</v>
       </c>
       <c r="J234" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K234" s="1" t="s">
         <v>876</v>
@@ -59351,7 +59355,7 @@
         <v>234</v>
       </c>
       <c r="J235" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K235" s="1" t="s">
         <v>876</v>
@@ -59380,7 +59384,7 @@
         <v>235</v>
       </c>
       <c r="J236" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K236" s="1" t="s">
         <v>876</v>
@@ -59409,7 +59413,7 @@
         <v>236</v>
       </c>
       <c r="J237" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K237" s="1" t="s">
         <v>876</v>
@@ -59438,7 +59442,7 @@
         <v>237</v>
       </c>
       <c r="J238" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K238" s="1" t="s">
         <v>876</v>
@@ -59467,7 +59471,7 @@
         <v>238</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K239" s="1" t="s">
         <v>876</v>
@@ -59499,7 +59503,7 @@
         <v>711</v>
       </c>
       <c r="J240" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K240" s="1" t="s">
         <v>876</v>
@@ -59531,7 +59535,7 @@
         <v>711</v>
       </c>
       <c r="J241" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K241" s="1" t="s">
         <v>876</v>
@@ -59563,7 +59567,7 @@
         <v>711</v>
       </c>
       <c r="J242" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K242" s="1" t="s">
         <v>876</v>
@@ -59595,7 +59599,7 @@
         <v>711</v>
       </c>
       <c r="J243" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K243" s="1" t="s">
         <v>876</v>
@@ -59627,7 +59631,7 @@
         <v>711</v>
       </c>
       <c r="J244" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K244" s="1" t="s">
         <v>876</v>
@@ -59656,7 +59660,7 @@
         <v>244</v>
       </c>
       <c r="J245" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K245" s="1" t="s">
         <v>876</v>
@@ -59685,7 +59689,7 @@
         <v>245</v>
       </c>
       <c r="J246" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K246" s="1" t="s">
         <v>876</v>
@@ -59714,7 +59718,7 @@
         <v>246</v>
       </c>
       <c r="J247" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K247" s="1" t="s">
         <v>876</v>
@@ -59746,7 +59750,7 @@
         <v>711</v>
       </c>
       <c r="J248" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K248" s="1" t="s">
         <v>876</v>
@@ -59778,7 +59782,7 @@
         <v>711</v>
       </c>
       <c r="J249" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K249" s="1" t="s">
         <v>876</v>
@@ -59810,7 +59814,7 @@
         <v>711</v>
       </c>
       <c r="J250" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K250" s="1" t="s">
         <v>876</v>
@@ -59842,7 +59846,7 @@
         <v>711</v>
       </c>
       <c r="J251" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K251" s="1" t="s">
         <v>876</v>
@@ -59874,7 +59878,7 @@
         <v>711</v>
       </c>
       <c r="J252" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K252" s="1" t="s">
         <v>876</v>
@@ -59906,7 +59910,7 @@
         <v>711</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K253" s="1" t="s">
         <v>876</v>
@@ -59938,7 +59942,7 @@
         <v>711</v>
       </c>
       <c r="J254" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K254" s="1" t="s">
         <v>876</v>
@@ -59967,7 +59971,7 @@
         <v>254</v>
       </c>
       <c r="J255" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K255" s="1" t="s">
         <v>876</v>
@@ -59996,7 +60000,7 @@
         <v>255</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K256" s="1" t="s">
         <v>876</v>
@@ -60028,7 +60032,7 @@
         <v>711</v>
       </c>
       <c r="J257" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K257" s="1" t="s">
         <v>876</v>
@@ -60060,7 +60064,7 @@
         <v>711</v>
       </c>
       <c r="J258" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K258" s="1" t="s">
         <v>876</v>
@@ -60092,7 +60096,7 @@
         <v>711</v>
       </c>
       <c r="J259" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K259" s="1" t="s">
         <v>876</v>
@@ -60124,7 +60128,7 @@
         <v>711</v>
       </c>
       <c r="J260" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K260" s="1" t="s">
         <v>876</v>
@@ -60156,7 +60160,7 @@
         <v>711</v>
       </c>
       <c r="J261" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K261" s="1" t="s">
         <v>876</v>
@@ -60188,7 +60192,7 @@
         <v>711</v>
       </c>
       <c r="J262" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K262" s="1" t="s">
         <v>876</v>
@@ -60220,7 +60224,7 @@
         <v>711</v>
       </c>
       <c r="J263" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K263" s="1" t="s">
         <v>876</v>
@@ -60252,7 +60256,7 @@
         <v>711</v>
       </c>
       <c r="J264" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K264" s="1" t="s">
         <v>876</v>
@@ -60284,7 +60288,7 @@
         <v>711</v>
       </c>
       <c r="J265" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K265" s="1" t="s">
         <v>876</v>
@@ -60316,7 +60320,7 @@
         <v>711</v>
       </c>
       <c r="J266" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K266" s="1" t="s">
         <v>876</v>
@@ -60345,7 +60349,7 @@
         <v>266</v>
       </c>
       <c r="J267" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K267" s="1" t="s">
         <v>876</v>
@@ -60374,7 +60378,7 @@
         <v>267</v>
       </c>
       <c r="J268" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K268" s="1" t="s">
         <v>876</v>
@@ -60406,7 +60410,7 @@
         <v>711</v>
       </c>
       <c r="J269" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K269" s="1" t="s">
         <v>876</v>
@@ -60438,7 +60442,7 @@
         <v>711</v>
       </c>
       <c r="J270" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K270" s="1" t="s">
         <v>876</v>
@@ -60470,7 +60474,7 @@
         <v>711</v>
       </c>
       <c r="J271" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K271" s="1" t="s">
         <v>876</v>
@@ -60502,7 +60506,7 @@
         <v>711</v>
       </c>
       <c r="J272" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K272" s="1" t="s">
         <v>876</v>
@@ -60534,7 +60538,7 @@
         <v>711</v>
       </c>
       <c r="J273" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K273" s="1" t="s">
         <v>876</v>
@@ -60566,7 +60570,7 @@
         <v>711</v>
       </c>
       <c r="J274" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K274" s="1" t="s">
         <v>876</v>
@@ -60598,7 +60602,7 @@
         <v>711</v>
       </c>
       <c r="J275" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K275" s="1" t="s">
         <v>876</v>
@@ -60630,7 +60634,7 @@
         <v>711</v>
       </c>
       <c r="J276" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K276" s="1" t="s">
         <v>876</v>
@@ -60659,7 +60663,7 @@
         <v>272</v>
       </c>
       <c r="J277" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K277" s="1" t="s">
         <v>876</v>
@@ -60688,7 +60692,7 @@
         <v>273</v>
       </c>
       <c r="J278" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K278" s="1" t="s">
         <v>876</v>
@@ -60717,7 +60721,7 @@
         <v>274</v>
       </c>
       <c r="J279" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K279" s="1" t="s">
         <v>876</v>
@@ -60746,7 +60750,7 @@
         <v>275</v>
       </c>
       <c r="J280" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K280" s="1" t="s">
         <v>876</v>
@@ -60775,7 +60779,7 @@
         <v>276</v>
       </c>
       <c r="J281" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K281" s="1" t="s">
         <v>876</v>
@@ -60804,7 +60808,7 @@
         <v>277</v>
       </c>
       <c r="J282" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K282" s="1" t="s">
         <v>876</v>
@@ -60833,7 +60837,7 @@
         <v>278</v>
       </c>
       <c r="J283" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K283" s="1" t="s">
         <v>876</v>
@@ -60865,7 +60869,7 @@
         <v>711</v>
       </c>
       <c r="J284" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K284" s="1" t="s">
         <v>876</v>
@@ -60897,7 +60901,7 @@
         <v>711</v>
       </c>
       <c r="J285" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K285" s="1" t="s">
         <v>876</v>
@@ -60926,7 +60930,7 @@
         <v>281</v>
       </c>
       <c r="J286" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K286" s="1" t="s">
         <v>876</v>
@@ -60955,7 +60959,7 @@
         <v>282</v>
       </c>
       <c r="J287" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K287" s="1" t="s">
         <v>876</v>
@@ -60984,7 +60988,7 @@
         <v>283</v>
       </c>
       <c r="J288" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K288" s="1" t="s">
         <v>876</v>
@@ -61013,7 +61017,7 @@
         <v>284</v>
       </c>
       <c r="J289" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K289" s="1" t="s">
         <v>876</v>
@@ -61042,7 +61046,7 @@
         <v>285</v>
       </c>
       <c r="J290" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K290" s="1" t="s">
         <v>876</v>
@@ -61071,7 +61075,7 @@
         <v>286</v>
       </c>
       <c r="J291" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K291" s="1" t="s">
         <v>876</v>
@@ -61100,7 +61104,7 @@
         <v>287</v>
       </c>
       <c r="J292" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K292" s="1" t="s">
         <v>876</v>
@@ -61129,7 +61133,7 @@
         <v>288</v>
       </c>
       <c r="J293" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K293" s="1" t="s">
         <v>876</v>
@@ -61161,7 +61165,7 @@
         <v>711</v>
       </c>
       <c r="J294" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K294" s="1" t="s">
         <v>876</v>
@@ -61193,7 +61197,7 @@
         <v>711</v>
       </c>
       <c r="J295" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K295" s="1" t="s">
         <v>876</v>
@@ -61222,7 +61226,7 @@
         <v>291</v>
       </c>
       <c r="J296" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K296" s="1" t="s">
         <v>876</v>
@@ -61251,7 +61255,7 @@
         <v>292</v>
       </c>
       <c r="J297" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K297" s="1" t="s">
         <v>876</v>
@@ -61280,7 +61284,7 @@
         <v>293</v>
       </c>
       <c r="J298" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K298" s="1" t="s">
         <v>876</v>
@@ -61312,7 +61316,7 @@
         <v>711</v>
       </c>
       <c r="J299" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K299" s="1" t="s">
         <v>876</v>
@@ -61344,7 +61348,7 @@
         <v>711</v>
       </c>
       <c r="J300" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K300" s="1" t="s">
         <v>876</v>
@@ -61373,7 +61377,7 @@
         <v>296</v>
       </c>
       <c r="J301" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K301" s="1" t="s">
         <v>876</v>
@@ -61402,7 +61406,7 @@
         <v>297</v>
       </c>
       <c r="J302" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K302" s="1" t="s">
         <v>876</v>
@@ -61434,7 +61438,7 @@
         <v>711</v>
       </c>
       <c r="J303" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K303" s="1" t="s">
         <v>876</v>
@@ -61463,7 +61467,7 @@
         <v>299</v>
       </c>
       <c r="J304" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K304" s="1" t="s">
         <v>876</v>
@@ -61492,7 +61496,7 @@
         <v>300</v>
       </c>
       <c r="J305" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K305" s="1" t="s">
         <v>876</v>
@@ -61521,7 +61525,7 @@
         <v>301</v>
       </c>
       <c r="J306" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K306" s="1" t="s">
         <v>876</v>
@@ -61553,7 +61557,7 @@
         <v>711</v>
       </c>
       <c r="J307" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K307" s="1" t="s">
         <v>876</v>
@@ -61582,7 +61586,7 @@
         <v>303</v>
       </c>
       <c r="J308" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K308" s="1" t="s">
         <v>876</v>
@@ -61614,7 +61618,7 @@
         <v>711</v>
       </c>
       <c r="J309" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K309" s="1" t="s">
         <v>876</v>
@@ -61643,7 +61647,7 @@
         <v>305</v>
       </c>
       <c r="J310" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K310" s="1" t="s">
         <v>876</v>
@@ -61675,7 +61679,7 @@
         <v>711</v>
       </c>
       <c r="J311" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K311" s="1" t="s">
         <v>876</v>
@@ -61704,7 +61708,7 @@
         <v>307</v>
       </c>
       <c r="J312" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K312" s="1" t="s">
         <v>876</v>
@@ -61733,7 +61737,7 @@
         <v>308</v>
       </c>
       <c r="J313" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K313" s="1" t="s">
         <v>876</v>
@@ -61765,7 +61769,7 @@
         <v>711</v>
       </c>
       <c r="J314" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K314" s="1" t="s">
         <v>876</v>
@@ -61797,7 +61801,7 @@
         <v>711</v>
       </c>
       <c r="J315" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K315" s="1" t="s">
         <v>876</v>
@@ -61829,7 +61833,7 @@
         <v>711</v>
       </c>
       <c r="J316" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K316" s="1" t="s">
         <v>876</v>
@@ -61861,7 +61865,7 @@
         <v>711</v>
       </c>
       <c r="J317" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K317" s="1" t="s">
         <v>876</v>
@@ -61893,7 +61897,7 @@
         <v>711</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K318" s="1" t="s">
         <v>876</v>
@@ -61925,7 +61929,7 @@
         <v>711</v>
       </c>
       <c r="J319" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K319" s="1" t="s">
         <v>876</v>
@@ -61957,7 +61961,7 @@
         <v>711</v>
       </c>
       <c r="J320" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K320" s="1" t="s">
         <v>876</v>
@@ -61986,7 +61990,7 @@
         <v>316</v>
       </c>
       <c r="J321" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K321" s="1" t="s">
         <v>1324</v>
@@ -62015,7 +62019,7 @@
         <v>317</v>
       </c>
       <c r="J322" s="4" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="K322" s="1" t="s">
         <v>1324</v>
@@ -62044,7 +62048,7 @@
         <v>318</v>
       </c>
       <c r="J323" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K323" s="1" t="s">
         <v>1324</v>
@@ -62073,7 +62077,7 @@
         <v>319</v>
       </c>
       <c r="J324" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K324" s="1" t="s">
         <v>1324</v>
@@ -62102,7 +62106,7 @@
         <v>320</v>
       </c>
       <c r="J325" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K325" s="1" t="s">
         <v>1324</v>
@@ -62131,7 +62135,7 @@
         <v>321</v>
       </c>
       <c r="J326" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K326" s="1" t="s">
         <v>1324</v>
@@ -62160,7 +62164,7 @@
         <v>322</v>
       </c>
       <c r="J327" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K327" s="1" t="s">
         <v>1324</v>
@@ -62189,7 +62193,7 @@
         <v>323</v>
       </c>
       <c r="J328" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K328" s="1" t="s">
         <v>1324</v>
@@ -62218,7 +62222,7 @@
         <v>324</v>
       </c>
       <c r="J329" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K329" s="1" t="s">
         <v>1324</v>
@@ -62247,7 +62251,7 @@
         <v>325</v>
       </c>
       <c r="J330" s="4" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="K330" s="1" t="s">
         <v>1324</v>
@@ -62276,7 +62280,7 @@
         <v>326</v>
       </c>
       <c r="J331" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K331" s="1" t="s">
         <v>1324</v>
@@ -62305,7 +62309,7 @@
         <v>327</v>
       </c>
       <c r="J332" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K332" s="1" t="s">
         <v>1324</v>
@@ -62334,7 +62338,7 @@
         <v>328</v>
       </c>
       <c r="J333" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K333" s="1" t="s">
         <v>1324</v>
@@ -62363,7 +62367,7 @@
         <v>329</v>
       </c>
       <c r="J334" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K334" s="1" t="s">
         <v>1324</v>
@@ -62392,7 +62396,7 @@
         <v>330</v>
       </c>
       <c r="J335" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K335" s="1" t="s">
         <v>1324</v>
@@ -62421,7 +62425,7 @@
         <v>331</v>
       </c>
       <c r="J336" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K336" s="1" t="s">
         <v>1324</v>
@@ -62450,7 +62454,7 @@
         <v>332</v>
       </c>
       <c r="J337" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K337" s="1" t="s">
         <v>1324</v>
@@ -62479,7 +62483,7 @@
         <v>333</v>
       </c>
       <c r="J338" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K338" s="1" t="s">
         <v>1324</v>
@@ -62508,7 +62512,7 @@
         <v>334</v>
       </c>
       <c r="J339" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K339" s="1" t="s">
         <v>1324</v>
@@ -62537,7 +62541,7 @@
         <v>335</v>
       </c>
       <c r="J340" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K340" s="1" t="s">
         <v>1324</v>
@@ -62566,7 +62570,7 @@
         <v>336</v>
       </c>
       <c r="J341" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K341" s="1" t="s">
         <v>1324</v>
@@ -62595,7 +62599,7 @@
         <v>337</v>
       </c>
       <c r="J342" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K342" s="1" t="s">
         <v>1324</v>
@@ -62624,7 +62628,7 @@
         <v>338</v>
       </c>
       <c r="J343" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K343" s="1" t="s">
         <v>1324</v>
@@ -62653,7 +62657,7 @@
         <v>339</v>
       </c>
       <c r="J344" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K344" s="1" t="s">
         <v>1324</v>
@@ -62682,7 +62686,7 @@
         <v>340</v>
       </c>
       <c r="J345" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K345" s="1" t="s">
         <v>1324</v>
@@ -62714,7 +62718,7 @@
         <v>711</v>
       </c>
       <c r="J346" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K346" s="1" t="s">
         <v>1324</v>
@@ -62743,7 +62747,7 @@
         <v>342</v>
       </c>
       <c r="J347" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K347" s="1" t="s">
         <v>1324</v>
@@ -62772,7 +62776,7 @@
         <v>343</v>
       </c>
       <c r="J348" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K348" s="1" t="s">
         <v>1324</v>
@@ -62801,7 +62805,7 @@
         <v>344</v>
       </c>
       <c r="J349" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K349" s="1" t="s">
         <v>1324</v>
@@ -62830,7 +62834,7 @@
         <v>345</v>
       </c>
       <c r="J350" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K350" s="1" t="s">
         <v>1324</v>
@@ -62859,7 +62863,7 @@
         <v>346</v>
       </c>
       <c r="J351" s="4" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="K351" s="1" t="s">
         <v>1324</v>
@@ -62888,7 +62892,7 @@
         <v>347</v>
       </c>
       <c r="J352" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K352" s="1" t="s">
         <v>1324</v>
@@ -62917,7 +62921,7 @@
         <v>348</v>
       </c>
       <c r="J353" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K353" s="1" t="s">
         <v>1324</v>
@@ -62946,7 +62950,7 @@
         <v>349</v>
       </c>
       <c r="J354" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K354" s="1" t="s">
         <v>1324</v>
@@ -62975,7 +62979,7 @@
         <v>350</v>
       </c>
       <c r="J355" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K355" s="1" t="s">
         <v>1324</v>
@@ -63004,7 +63008,7 @@
         <v>351</v>
       </c>
       <c r="J356" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K356" s="1" t="s">
         <v>1324</v>
@@ -63033,7 +63037,7 @@
         <v>352</v>
       </c>
       <c r="J357" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K357" s="1" t="s">
         <v>1324</v>
@@ -63065,7 +63069,7 @@
         <v>711</v>
       </c>
       <c r="J358" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K358" s="1" t="s">
         <v>1324</v>
@@ -63094,7 +63098,7 @@
         <v>354</v>
       </c>
       <c r="J359" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K359" s="1" t="s">
         <v>1324</v>
@@ -63123,7 +63127,7 @@
         <v>355</v>
       </c>
       <c r="J360" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K360" s="1" t="s">
         <v>1324</v>
@@ -63152,13 +63156,14 @@
         <v>356</v>
       </c>
       <c r="J361" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="K361" s="1" t="s">
         <v>1324</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K361" xr:uid="{C9791905-45CB-4A13-A607-A158D8B6240A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v0.4.0 -- important advance in app functionality and figure coordination.
</commit_message>
<xml_diff>
--- a/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
+++ b/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpascariu\Documents\R-Repos\MortalityCauses\data-raw\GBD_2019_Data_Tools_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0A2F04-1C00-444E-87D0-B41FDDDB9215}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1484A5-3EFA-48E2-818D-57EE401BF1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4647" uniqueCount="1615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4647" uniqueCount="1617">
   <si>
     <t>Global</t>
   </si>
@@ -4852,9 +4852,6 @@
     <t>app_selection</t>
   </si>
   <si>
-    <t>Other Non-Communicable Diseases</t>
-  </si>
-  <si>
     <t>Lung cancer</t>
   </si>
   <si>
@@ -4867,14 +4864,22 @@
     <t>Communicable Diseases</t>
   </si>
   <si>
-    <t>Injuries: Self-harm and Violence</t>
-  </si>
-  <si>
-    <t>Injuries: Transport and Unintentional</t>
-  </si>
-  <si>
-    <t>Other Communicable Diseases: 
-infections and nutritional deficiencies</t>
+    <t>HIV/ AIDS / STD</t>
+  </si>
+  <si>
+    <t>Infections</t>
+  </si>
+  <si>
+    <t>Self-harm and Violence</t>
+  </si>
+  <si>
+    <t>Other cardiovascular</t>
+  </si>
+  <si>
+    <t>Respiratory infections</t>
+  </si>
+  <si>
+    <t>Other Non-Communicable</t>
   </si>
 </sst>
 </file>
@@ -5388,7 +5393,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -52403,9 +52408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52455,7 +52460,7 @@
         <v>1606</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -52481,10 +52486,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -52510,10 +52515,10 @@
         <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -52538,11 +52543,11 @@
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>689</v>
+      <c r="J4" t="s">
+        <v>1611</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -52568,10 +52573,10 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -52597,10 +52602,10 @@
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -52626,10 +52631,10 @@
         <v>6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -52655,10 +52660,10 @@
         <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -52684,10 +52689,10 @@
         <v>8</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -52713,10 +52718,10 @@
         <v>9</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -52742,10 +52747,10 @@
         <v>10</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -52771,10 +52776,10 @@
         <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -52800,10 +52805,10 @@
         <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -52832,10 +52837,10 @@
         <v>711</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -52864,10 +52869,10 @@
         <v>711</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -52893,10 +52898,10 @@
         <v>15</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -52922,10 +52927,10 @@
         <v>16</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>716</v>
+        <v>1615</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -52951,10 +52956,10 @@
         <v>17</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -52983,10 +52988,10 @@
         <v>711</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -53012,10 +53017,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -53041,10 +53046,10 @@
         <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -53070,10 +53075,10 @@
         <v>21</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -53099,10 +53104,10 @@
         <v>22</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -53128,10 +53133,10 @@
         <v>23</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -53157,13 +53162,13 @@
         <v>24</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>957</v>
       </c>
@@ -53186,10 +53191,10 @@
         <v>25</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -53215,10 +53220,10 @@
         <v>26</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -53244,10 +53249,10 @@
         <v>27</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -53273,10 +53278,10 @@
         <v>28</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -53302,10 +53307,10 @@
         <v>29</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -53331,10 +53336,10 @@
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -53360,13 +53365,13 @@
         <v>31</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>344</v>
       </c>
@@ -53389,10 +53394,10 @@
         <v>32</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -53418,10 +53423,10 @@
         <v>33</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -53447,10 +53452,10 @@
         <v>34</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -53476,10 +53481,10 @@
         <v>35</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -53505,10 +53510,10 @@
         <v>36</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -53537,10 +53542,10 @@
         <v>711</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -53566,10 +53571,10 @@
         <v>38</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -53595,10 +53600,10 @@
         <v>39</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -53624,10 +53629,10 @@
         <v>40</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -53653,10 +53658,10 @@
         <v>41</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -53685,10 +53690,10 @@
         <v>711</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -53717,10 +53722,10 @@
         <v>711</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -53749,10 +53754,10 @@
         <v>711</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -53778,10 +53783,10 @@
         <v>45</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -53807,10 +53812,10 @@
         <v>46</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -53836,10 +53841,10 @@
         <v>47</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -53865,10 +53870,10 @@
         <v>48</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -53894,10 +53899,10 @@
         <v>49</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -53926,10 +53931,10 @@
         <v>711</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -53958,10 +53963,10 @@
         <v>711</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -53990,10 +53995,10 @@
         <v>711</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -54022,10 +54027,10 @@
         <v>711</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -54051,10 +54056,10 @@
         <v>54</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -54080,10 +54085,10 @@
         <v>55</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -54112,10 +54117,10 @@
         <v>711</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -54141,13 +54146,13 @@
         <v>57</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>961</v>
       </c>
@@ -54170,10 +54175,10 @@
         <v>58</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -54199,10 +54204,10 @@
         <v>59</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -54228,10 +54233,10 @@
         <v>60</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -54257,10 +54262,10 @@
         <v>61</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -54286,10 +54291,10 @@
         <v>62</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -54315,10 +54320,10 @@
         <v>63</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -54344,10 +54349,10 @@
         <v>64</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -54373,10 +54378,10 @@
         <v>65</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -54402,10 +54407,10 @@
         <v>66</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -54431,10 +54436,10 @@
         <v>67</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -54460,10 +54465,10 @@
         <v>68</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -54489,10 +54494,10 @@
         <v>69</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -54518,10 +54523,10 @@
         <v>70</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -54547,10 +54552,10 @@
         <v>71</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -54576,10 +54581,10 @@
         <v>72</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>828</v>
+        <v>852</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -54605,10 +54610,10 @@
         <v>73</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -54634,10 +54639,10 @@
         <v>74</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -54663,10 +54668,10 @@
         <v>75</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -54692,10 +54697,10 @@
         <v>76</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -54721,10 +54726,10 @@
         <v>77</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -54750,10 +54755,10 @@
         <v>78</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -54779,10 +54784,10 @@
         <v>79</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -54811,10 +54816,10 @@
         <v>711</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -54843,10 +54848,10 @@
         <v>711</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -54875,10 +54880,10 @@
         <v>711</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -54904,10 +54909,10 @@
         <v>83</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -54933,10 +54938,10 @@
         <v>84</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -54962,10 +54967,10 @@
         <v>85</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -54991,10 +54996,10 @@
         <v>86</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -55020,10 +55025,10 @@
         <v>87</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -55049,10 +55054,10 @@
         <v>88</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -55078,13 +55083,13 @@
         <v>89</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>386</v>
       </c>
@@ -55107,10 +55112,10 @@
         <v>90</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -55136,10 +55141,10 @@
         <v>91</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -55168,10 +55173,10 @@
         <v>711</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -55200,10 +55205,10 @@
         <v>711</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -55232,10 +55237,10 @@
         <v>711</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -55261,10 +55266,10 @@
         <v>95</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -55290,7 +55295,7 @@
         <v>96</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>876</v>
@@ -55319,7 +55324,7 @@
         <v>97</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>876</v>
@@ -55551,7 +55556,7 @@
         <v>105</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>876</v>
@@ -55580,7 +55585,7 @@
         <v>106</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>876</v>
@@ -55609,7 +55614,7 @@
         <v>107</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>876</v>
@@ -55638,7 +55643,7 @@
         <v>108</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>876</v>
@@ -55667,7 +55672,7 @@
         <v>109</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>876</v>
@@ -55783,7 +55788,7 @@
         <v>113</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>876</v>
@@ -55870,7 +55875,7 @@
         <v>116</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>876</v>
@@ -55902,7 +55907,7 @@
         <v>711</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>876</v>
@@ -56366,7 +56371,7 @@
         <v>133</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>876</v>
@@ -56395,7 +56400,7 @@
         <v>134</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K135" s="1" t="s">
         <v>876</v>
@@ -56424,7 +56429,7 @@
         <v>135</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K136" s="1" t="s">
         <v>876</v>
@@ -56453,7 +56458,7 @@
         <v>136</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K137" s="1" t="s">
         <v>876</v>
@@ -56482,7 +56487,7 @@
         <v>137</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>876</v>
@@ -56569,7 +56574,7 @@
         <v>140</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K141" s="1" t="s">
         <v>876</v>
@@ -56601,7 +56606,7 @@
         <v>711</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K142" s="1" t="s">
         <v>876</v>
@@ -56633,7 +56638,7 @@
         <v>711</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K143" s="1" t="s">
         <v>876</v>
@@ -56665,7 +56670,7 @@
         <v>711</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K144" s="1" t="s">
         <v>876</v>
@@ -56694,7 +56699,7 @@
         <v>144</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K145" s="1" t="s">
         <v>876</v>
@@ -56723,7 +56728,7 @@
         <v>145</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K146" s="1" t="s">
         <v>876</v>
@@ -56810,7 +56815,7 @@
         <v>148</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>876</v>
@@ -56839,7 +56844,7 @@
         <v>149</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>876</v>
@@ -56868,7 +56873,7 @@
         <v>150</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K151" s="1" t="s">
         <v>876</v>
@@ -56897,7 +56902,7 @@
         <v>151</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K152" s="1" t="s">
         <v>876</v>
@@ -56926,7 +56931,7 @@
         <v>152</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K153" s="1" t="s">
         <v>876</v>
@@ -56955,7 +56960,7 @@
         <v>153</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>876</v>
@@ -56984,7 +56989,7 @@
         <v>154</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K155" s="1" t="s">
         <v>876</v>
@@ -57013,7 +57018,7 @@
         <v>155</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>876</v>
@@ -57042,7 +57047,7 @@
         <v>156</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K157" s="1" t="s">
         <v>876</v>
@@ -57071,7 +57076,7 @@
         <v>157</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>876</v>
@@ -57100,7 +57105,7 @@
         <v>158</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K159" s="1" t="s">
         <v>876</v>
@@ -57129,7 +57134,7 @@
         <v>159</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>876</v>
@@ -57158,7 +57163,7 @@
         <v>160</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K161" s="1" t="s">
         <v>876</v>
@@ -57190,7 +57195,7 @@
         <v>711</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K162" s="1" t="s">
         <v>876</v>
@@ -57219,7 +57224,7 @@
         <v>162</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>876</v>
@@ -57248,7 +57253,7 @@
         <v>163</v>
       </c>
       <c r="J164" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K164" s="1" t="s">
         <v>876</v>
@@ -57277,7 +57282,7 @@
         <v>164</v>
       </c>
       <c r="J165" s="2" t="s">
-        <v>1012</v>
+        <v>1614</v>
       </c>
       <c r="K165" s="1" t="s">
         <v>876</v>
@@ -57335,7 +57340,7 @@
         <v>166</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K167" s="1" t="s">
         <v>876</v>
@@ -57364,7 +57369,7 @@
         <v>167</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K168" s="1" t="s">
         <v>876</v>
@@ -57393,7 +57398,7 @@
         <v>168</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K169" s="1" t="s">
         <v>876</v>
@@ -57422,7 +57427,7 @@
         <v>169</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K170" s="1" t="s">
         <v>876</v>
@@ -57451,7 +57456,7 @@
         <v>170</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K171" s="1" t="s">
         <v>876</v>
@@ -57480,7 +57485,7 @@
         <v>171</v>
       </c>
       <c r="J172" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K172" s="1" t="s">
         <v>876</v>
@@ -57509,7 +57514,7 @@
         <v>172</v>
       </c>
       <c r="J173" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K173" s="1" t="s">
         <v>876</v>
@@ -57538,7 +57543,7 @@
         <v>173</v>
       </c>
       <c r="J174" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K174" s="1" t="s">
         <v>876</v>
@@ -57567,7 +57572,7 @@
         <v>174</v>
       </c>
       <c r="J175" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K175" s="1" t="s">
         <v>876</v>
@@ -57625,7 +57630,7 @@
         <v>176</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K177" s="1" t="s">
         <v>876</v>
@@ -57654,7 +57659,7 @@
         <v>177</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K178" s="1" t="s">
         <v>876</v>
@@ -57683,7 +57688,7 @@
         <v>178</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K179" s="1" t="s">
         <v>876</v>
@@ -57712,7 +57717,7 @@
         <v>179</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K180" s="1" t="s">
         <v>876</v>
@@ -57741,7 +57746,7 @@
         <v>180</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K181" s="1" t="s">
         <v>876</v>
@@ -57770,7 +57775,7 @@
         <v>181</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K182" s="1" t="s">
         <v>876</v>
@@ -57799,7 +57804,7 @@
         <v>182</v>
       </c>
       <c r="J183" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K183" s="1" t="s">
         <v>876</v>
@@ -57828,7 +57833,7 @@
         <v>183</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K184" s="1" t="s">
         <v>876</v>
@@ -57857,7 +57862,7 @@
         <v>184</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K185" s="1" t="s">
         <v>876</v>
@@ -57889,7 +57894,7 @@
         <v>711</v>
       </c>
       <c r="J186" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K186" s="1" t="s">
         <v>876</v>
@@ -57918,7 +57923,7 @@
         <v>186</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K187" s="1" t="s">
         <v>876</v>
@@ -57947,7 +57952,7 @@
         <v>187</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K188" s="1" t="s">
         <v>876</v>
@@ -57976,7 +57981,7 @@
         <v>188</v>
       </c>
       <c r="J189" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K189" s="1" t="s">
         <v>876</v>
@@ -58005,7 +58010,7 @@
         <v>189</v>
       </c>
       <c r="J190" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K190" s="1" t="s">
         <v>876</v>
@@ -58034,7 +58039,7 @@
         <v>190</v>
       </c>
       <c r="J191" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K191" s="1" t="s">
         <v>876</v>
@@ -58063,7 +58068,7 @@
         <v>191</v>
       </c>
       <c r="J192" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K192" s="1" t="s">
         <v>876</v>
@@ -58092,7 +58097,7 @@
         <v>192</v>
       </c>
       <c r="J193" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K193" s="1" t="s">
         <v>876</v>
@@ -58121,7 +58126,7 @@
         <v>193</v>
       </c>
       <c r="J194" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K194" s="1" t="s">
         <v>876</v>
@@ -58179,7 +58184,7 @@
         <v>195</v>
       </c>
       <c r="J196" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K196" s="1" t="s">
         <v>876</v>
@@ -58208,7 +58213,7 @@
         <v>196</v>
       </c>
       <c r="J197" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K197" s="1" t="s">
         <v>876</v>
@@ -58237,7 +58242,7 @@
         <v>197</v>
       </c>
       <c r="J198" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K198" s="1" t="s">
         <v>876</v>
@@ -58266,7 +58271,7 @@
         <v>198</v>
       </c>
       <c r="J199" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K199" s="1" t="s">
         <v>876</v>
@@ -58295,7 +58300,7 @@
         <v>199</v>
       </c>
       <c r="J200" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K200" s="1" t="s">
         <v>876</v>
@@ -58327,7 +58332,7 @@
         <v>711</v>
       </c>
       <c r="J201" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K201" s="1" t="s">
         <v>876</v>
@@ -58359,7 +58364,7 @@
         <v>711</v>
       </c>
       <c r="J202" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K202" s="1" t="s">
         <v>876</v>
@@ -58391,7 +58396,7 @@
         <v>711</v>
       </c>
       <c r="J203" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K203" s="1" t="s">
         <v>876</v>
@@ -58420,7 +58425,7 @@
         <v>203</v>
       </c>
       <c r="J204" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K204" s="1" t="s">
         <v>876</v>
@@ -58449,7 +58454,7 @@
         <v>204</v>
       </c>
       <c r="J205" s="4" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="K205" s="1" t="s">
         <v>876</v>
@@ -58481,7 +58486,7 @@
         <v>711</v>
       </c>
       <c r="J206" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K206" s="1" t="s">
         <v>876</v>
@@ -58513,7 +58518,7 @@
         <v>711</v>
       </c>
       <c r="J207" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K207" s="1" t="s">
         <v>876</v>
@@ -58545,7 +58550,7 @@
         <v>711</v>
       </c>
       <c r="J208" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K208" s="1" t="s">
         <v>876</v>
@@ -58577,7 +58582,7 @@
         <v>711</v>
       </c>
       <c r="J209" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K209" s="1" t="s">
         <v>876</v>
@@ -58609,7 +58614,7 @@
         <v>711</v>
       </c>
       <c r="J210" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K210" s="1" t="s">
         <v>876</v>
@@ -58641,7 +58646,7 @@
         <v>711</v>
       </c>
       <c r="J211" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K211" s="1" t="s">
         <v>876</v>
@@ -58670,7 +58675,7 @@
         <v>211</v>
       </c>
       <c r="J212" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K212" s="1" t="s">
         <v>876</v>
@@ -58699,7 +58704,7 @@
         <v>212</v>
       </c>
       <c r="J213" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K213" s="1" t="s">
         <v>876</v>
@@ -58728,7 +58733,7 @@
         <v>213</v>
       </c>
       <c r="J214" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K214" s="1" t="s">
         <v>876</v>
@@ -58760,7 +58765,7 @@
         <v>711</v>
       </c>
       <c r="J215" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K215" s="1" t="s">
         <v>876</v>
@@ -58792,7 +58797,7 @@
         <v>711</v>
       </c>
       <c r="J216" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K216" s="1" t="s">
         <v>876</v>
@@ -58824,7 +58829,7 @@
         <v>711</v>
       </c>
       <c r="J217" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K217" s="1" t="s">
         <v>876</v>
@@ -58856,7 +58861,7 @@
         <v>711</v>
       </c>
       <c r="J218" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K218" s="1" t="s">
         <v>876</v>
@@ -58888,7 +58893,7 @@
         <v>711</v>
       </c>
       <c r="J219" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K219" s="1" t="s">
         <v>876</v>
@@ -58917,7 +58922,7 @@
         <v>219</v>
       </c>
       <c r="J220" s="4" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="K220" s="1" t="s">
         <v>876</v>
@@ -58946,7 +58951,7 @@
         <v>220</v>
       </c>
       <c r="J221" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K221" s="1" t="s">
         <v>876</v>
@@ -58975,7 +58980,7 @@
         <v>221</v>
       </c>
       <c r="J222" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K222" s="1" t="s">
         <v>876</v>
@@ -59004,7 +59009,7 @@
         <v>222</v>
       </c>
       <c r="J223" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K223" s="1" t="s">
         <v>876</v>
@@ -59033,7 +59038,7 @@
         <v>223</v>
       </c>
       <c r="J224" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K224" s="1" t="s">
         <v>876</v>
@@ -59062,7 +59067,7 @@
         <v>224</v>
       </c>
       <c r="J225" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K225" s="1" t="s">
         <v>876</v>
@@ -59094,7 +59099,7 @@
         <v>711</v>
       </c>
       <c r="J226" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K226" s="1" t="s">
         <v>876</v>
@@ -59123,7 +59128,7 @@
         <v>226</v>
       </c>
       <c r="J227" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K227" s="1" t="s">
         <v>876</v>
@@ -59181,7 +59186,7 @@
         <v>228</v>
       </c>
       <c r="J229" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K229" s="1" t="s">
         <v>876</v>
@@ -59210,7 +59215,7 @@
         <v>229</v>
       </c>
       <c r="J230" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K230" s="1" t="s">
         <v>876</v>
@@ -59239,7 +59244,7 @@
         <v>230</v>
       </c>
       <c r="J231" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K231" s="1" t="s">
         <v>876</v>
@@ -59268,7 +59273,7 @@
         <v>231</v>
       </c>
       <c r="J232" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K232" s="1" t="s">
         <v>876</v>
@@ -59297,7 +59302,7 @@
         <v>232</v>
       </c>
       <c r="J233" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K233" s="1" t="s">
         <v>876</v>
@@ -59326,7 +59331,7 @@
         <v>233</v>
       </c>
       <c r="J234" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K234" s="1" t="s">
         <v>876</v>
@@ -59355,7 +59360,7 @@
         <v>234</v>
       </c>
       <c r="J235" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K235" s="1" t="s">
         <v>876</v>
@@ -59384,7 +59389,7 @@
         <v>235</v>
       </c>
       <c r="J236" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K236" s="1" t="s">
         <v>876</v>
@@ -59413,7 +59418,7 @@
         <v>236</v>
       </c>
       <c r="J237" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K237" s="1" t="s">
         <v>876</v>
@@ -59442,7 +59447,7 @@
         <v>237</v>
       </c>
       <c r="J238" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K238" s="1" t="s">
         <v>876</v>
@@ -59471,7 +59476,7 @@
         <v>238</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="K239" s="1" t="s">
         <v>876</v>
@@ -59503,7 +59508,7 @@
         <v>711</v>
       </c>
       <c r="J240" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K240" s="1" t="s">
         <v>876</v>
@@ -59535,7 +59540,7 @@
         <v>711</v>
       </c>
       <c r="J241" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K241" s="1" t="s">
         <v>876</v>
@@ -59567,7 +59572,7 @@
         <v>711</v>
       </c>
       <c r="J242" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K242" s="1" t="s">
         <v>876</v>
@@ -59599,7 +59604,7 @@
         <v>711</v>
       </c>
       <c r="J243" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K243" s="1" t="s">
         <v>876</v>
@@ -59631,7 +59636,7 @@
         <v>711</v>
       </c>
       <c r="J244" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K244" s="1" t="s">
         <v>876</v>
@@ -59660,7 +59665,7 @@
         <v>244</v>
       </c>
       <c r="J245" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K245" s="1" t="s">
         <v>876</v>
@@ -59689,7 +59694,7 @@
         <v>245</v>
       </c>
       <c r="J246" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K246" s="1" t="s">
         <v>876</v>
@@ -59718,7 +59723,7 @@
         <v>246</v>
       </c>
       <c r="J247" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K247" s="1" t="s">
         <v>876</v>
@@ -59750,7 +59755,7 @@
         <v>711</v>
       </c>
       <c r="J248" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K248" s="1" t="s">
         <v>876</v>
@@ -59782,7 +59787,7 @@
         <v>711</v>
       </c>
       <c r="J249" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K249" s="1" t="s">
         <v>876</v>
@@ -59814,7 +59819,7 @@
         <v>711</v>
       </c>
       <c r="J250" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K250" s="1" t="s">
         <v>876</v>
@@ -59846,7 +59851,7 @@
         <v>711</v>
       </c>
       <c r="J251" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K251" s="1" t="s">
         <v>876</v>
@@ -59878,7 +59883,7 @@
         <v>711</v>
       </c>
       <c r="J252" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K252" s="1" t="s">
         <v>876</v>
@@ -59910,7 +59915,7 @@
         <v>711</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K253" s="1" t="s">
         <v>876</v>
@@ -59942,7 +59947,7 @@
         <v>711</v>
       </c>
       <c r="J254" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K254" s="1" t="s">
         <v>876</v>
@@ -59971,7 +59976,7 @@
         <v>254</v>
       </c>
       <c r="J255" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K255" s="1" t="s">
         <v>876</v>
@@ -60000,7 +60005,7 @@
         <v>255</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K256" s="1" t="s">
         <v>876</v>
@@ -60032,7 +60037,7 @@
         <v>711</v>
       </c>
       <c r="J257" s="4" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="K257" s="1" t="s">
         <v>876</v>
@@ -60064,7 +60069,7 @@
         <v>711</v>
       </c>
       <c r="J258" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K258" s="1" t="s">
         <v>876</v>
@@ -60096,7 +60101,7 @@
         <v>711</v>
       </c>
       <c r="J259" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K259" s="1" t="s">
         <v>876</v>
@@ -60128,7 +60133,7 @@
         <v>711</v>
       </c>
       <c r="J260" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K260" s="1" t="s">
         <v>876</v>
@@ -60160,7 +60165,7 @@
         <v>711</v>
       </c>
       <c r="J261" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K261" s="1" t="s">
         <v>876</v>
@@ -60192,7 +60197,7 @@
         <v>711</v>
       </c>
       <c r="J262" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K262" s="1" t="s">
         <v>876</v>
@@ -60224,7 +60229,7 @@
         <v>711</v>
       </c>
       <c r="J263" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K263" s="1" t="s">
         <v>876</v>
@@ -60256,7 +60261,7 @@
         <v>711</v>
       </c>
       <c r="J264" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K264" s="1" t="s">
         <v>876</v>
@@ -60288,7 +60293,7 @@
         <v>711</v>
       </c>
       <c r="J265" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K265" s="1" t="s">
         <v>876</v>
@@ -60320,7 +60325,7 @@
         <v>711</v>
       </c>
       <c r="J266" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K266" s="1" t="s">
         <v>876</v>
@@ -60349,7 +60354,7 @@
         <v>266</v>
       </c>
       <c r="J267" s="4" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="K267" s="1" t="s">
         <v>876</v>
@@ -60378,7 +60383,7 @@
         <v>267</v>
       </c>
       <c r="J268" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K268" s="1" t="s">
         <v>876</v>
@@ -60410,7 +60415,7 @@
         <v>711</v>
       </c>
       <c r="J269" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K269" s="1" t="s">
         <v>876</v>
@@ -60442,7 +60447,7 @@
         <v>711</v>
       </c>
       <c r="J270" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K270" s="1" t="s">
         <v>876</v>
@@ -60474,7 +60479,7 @@
         <v>711</v>
       </c>
       <c r="J271" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K271" s="1" t="s">
         <v>876</v>
@@ -60506,7 +60511,7 @@
         <v>711</v>
       </c>
       <c r="J272" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K272" s="1" t="s">
         <v>876</v>
@@ -60538,7 +60543,7 @@
         <v>711</v>
       </c>
       <c r="J273" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K273" s="1" t="s">
         <v>876</v>
@@ -60570,7 +60575,7 @@
         <v>711</v>
       </c>
       <c r="J274" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K274" s="1" t="s">
         <v>876</v>
@@ -60602,7 +60607,7 @@
         <v>711</v>
       </c>
       <c r="J275" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K275" s="1" t="s">
         <v>876</v>
@@ -60634,7 +60639,7 @@
         <v>711</v>
       </c>
       <c r="J276" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K276" s="1" t="s">
         <v>876</v>
@@ -60663,7 +60668,7 @@
         <v>272</v>
       </c>
       <c r="J277" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K277" s="1" t="s">
         <v>876</v>
@@ -60692,7 +60697,7 @@
         <v>273</v>
       </c>
       <c r="J278" s="4" t="s">
-        <v>1607</v>
+        <v>1616</v>
       </c>
       <c r="K278" s="1" t="s">
         <v>876</v>
@@ -60721,7 +60726,7 @@
         <v>274</v>
       </c>
       <c r="J279" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K279" s="1" t="s">
         <v>876</v>
@@ -60750,7 +60755,7 @@
         <v>275</v>
       </c>
       <c r="J280" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K280" s="1" t="s">
         <v>876</v>
@@ -60779,7 +60784,7 @@
         <v>276</v>
       </c>
       <c r="J281" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K281" s="1" t="s">
         <v>876</v>
@@ -60808,7 +60813,7 @@
         <v>277</v>
       </c>
       <c r="J282" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K282" s="1" t="s">
         <v>876</v>
@@ -60837,7 +60842,7 @@
         <v>278</v>
       </c>
       <c r="J283" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K283" s="1" t="s">
         <v>876</v>
@@ -60869,7 +60874,7 @@
         <v>711</v>
       </c>
       <c r="J284" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K284" s="1" t="s">
         <v>876</v>
@@ -60901,7 +60906,7 @@
         <v>711</v>
       </c>
       <c r="J285" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K285" s="1" t="s">
         <v>876</v>
@@ -60930,7 +60935,7 @@
         <v>281</v>
       </c>
       <c r="J286" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K286" s="1" t="s">
         <v>876</v>
@@ -60959,7 +60964,7 @@
         <v>282</v>
       </c>
       <c r="J287" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K287" s="1" t="s">
         <v>876</v>
@@ -60988,7 +60993,7 @@
         <v>283</v>
       </c>
       <c r="J288" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K288" s="1" t="s">
         <v>876</v>
@@ -61017,7 +61022,7 @@
         <v>284</v>
       </c>
       <c r="J289" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K289" s="1" t="s">
         <v>876</v>
@@ -61046,7 +61051,7 @@
         <v>285</v>
       </c>
       <c r="J290" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K290" s="1" t="s">
         <v>876</v>
@@ -61075,7 +61080,7 @@
         <v>286</v>
       </c>
       <c r="J291" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K291" s="1" t="s">
         <v>876</v>
@@ -61104,7 +61109,7 @@
         <v>287</v>
       </c>
       <c r="J292" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K292" s="1" t="s">
         <v>876</v>
@@ -61133,7 +61138,7 @@
         <v>288</v>
       </c>
       <c r="J293" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K293" s="1" t="s">
         <v>876</v>
@@ -61165,7 +61170,7 @@
         <v>711</v>
       </c>
       <c r="J294" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K294" s="1" t="s">
         <v>876</v>
@@ -61197,7 +61202,7 @@
         <v>711</v>
       </c>
       <c r="J295" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K295" s="1" t="s">
         <v>876</v>
@@ -61226,7 +61231,7 @@
         <v>291</v>
       </c>
       <c r="J296" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K296" s="1" t="s">
         <v>876</v>
@@ -61255,7 +61260,7 @@
         <v>292</v>
       </c>
       <c r="J297" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K297" s="1" t="s">
         <v>876</v>
@@ -61284,7 +61289,7 @@
         <v>293</v>
       </c>
       <c r="J298" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K298" s="1" t="s">
         <v>876</v>
@@ -61316,7 +61321,7 @@
         <v>711</v>
       </c>
       <c r="J299" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K299" s="1" t="s">
         <v>876</v>
@@ -61348,7 +61353,7 @@
         <v>711</v>
       </c>
       <c r="J300" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K300" s="1" t="s">
         <v>876</v>
@@ -61377,7 +61382,7 @@
         <v>296</v>
       </c>
       <c r="J301" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K301" s="1" t="s">
         <v>876</v>
@@ -61406,7 +61411,7 @@
         <v>297</v>
       </c>
       <c r="J302" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K302" s="1" t="s">
         <v>876</v>
@@ -61438,7 +61443,7 @@
         <v>711</v>
       </c>
       <c r="J303" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K303" s="1" t="s">
         <v>876</v>
@@ -61467,7 +61472,7 @@
         <v>299</v>
       </c>
       <c r="J304" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K304" s="1" t="s">
         <v>876</v>
@@ -61496,7 +61501,7 @@
         <v>300</v>
       </c>
       <c r="J305" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K305" s="1" t="s">
         <v>876</v>
@@ -61525,7 +61530,7 @@
         <v>301</v>
       </c>
       <c r="J306" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K306" s="1" t="s">
         <v>876</v>
@@ -61557,7 +61562,7 @@
         <v>711</v>
       </c>
       <c r="J307" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K307" s="1" t="s">
         <v>876</v>
@@ -61586,7 +61591,7 @@
         <v>303</v>
       </c>
       <c r="J308" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K308" s="1" t="s">
         <v>876</v>
@@ -61618,7 +61623,7 @@
         <v>711</v>
       </c>
       <c r="J309" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K309" s="1" t="s">
         <v>876</v>
@@ -61647,7 +61652,7 @@
         <v>305</v>
       </c>
       <c r="J310" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K310" s="1" t="s">
         <v>876</v>
@@ -61679,7 +61684,7 @@
         <v>711</v>
       </c>
       <c r="J311" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K311" s="1" t="s">
         <v>876</v>
@@ -61708,7 +61713,7 @@
         <v>307</v>
       </c>
       <c r="J312" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K312" s="1" t="s">
         <v>876</v>
@@ -61737,7 +61742,7 @@
         <v>308</v>
       </c>
       <c r="J313" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K313" s="1" t="s">
         <v>876</v>
@@ -61769,7 +61774,7 @@
         <v>711</v>
       </c>
       <c r="J314" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K314" s="1" t="s">
         <v>876</v>
@@ -61801,7 +61806,7 @@
         <v>711</v>
       </c>
       <c r="J315" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K315" s="1" t="s">
         <v>876</v>
@@ -61833,7 +61838,7 @@
         <v>711</v>
       </c>
       <c r="J316" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K316" s="1" t="s">
         <v>876</v>
@@ -61865,7 +61870,7 @@
         <v>711</v>
       </c>
       <c r="J317" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K317" s="1" t="s">
         <v>876</v>
@@ -61897,7 +61902,7 @@
         <v>711</v>
       </c>
       <c r="J318" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K318" s="1" t="s">
         <v>876</v>
@@ -61929,7 +61934,7 @@
         <v>711</v>
       </c>
       <c r="J319" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K319" s="1" t="s">
         <v>876</v>
@@ -61961,7 +61966,7 @@
         <v>711</v>
       </c>
       <c r="J320" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K320" s="1" t="s">
         <v>876</v>
@@ -61990,7 +61995,7 @@
         <v>316</v>
       </c>
       <c r="J321" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K321" s="1" t="s">
         <v>1324</v>
@@ -62019,7 +62024,7 @@
         <v>317</v>
       </c>
       <c r="J322" s="4" t="s">
-        <v>1613</v>
+        <v>1324</v>
       </c>
       <c r="K322" s="1" t="s">
         <v>1324</v>
@@ -62048,7 +62053,7 @@
         <v>318</v>
       </c>
       <c r="J323" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K323" s="1" t="s">
         <v>1324</v>
@@ -62077,7 +62082,7 @@
         <v>319</v>
       </c>
       <c r="J324" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K324" s="1" t="s">
         <v>1324</v>
@@ -62106,7 +62111,7 @@
         <v>320</v>
       </c>
       <c r="J325" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K325" s="1" t="s">
         <v>1324</v>
@@ -62135,7 +62140,7 @@
         <v>321</v>
       </c>
       <c r="J326" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K326" s="1" t="s">
         <v>1324</v>
@@ -62164,7 +62169,7 @@
         <v>322</v>
       </c>
       <c r="J327" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K327" s="1" t="s">
         <v>1324</v>
@@ -62193,7 +62198,7 @@
         <v>323</v>
       </c>
       <c r="J328" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K328" s="1" t="s">
         <v>1324</v>
@@ -62222,7 +62227,7 @@
         <v>324</v>
       </c>
       <c r="J329" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K329" s="1" t="s">
         <v>1324</v>
@@ -62251,7 +62256,7 @@
         <v>325</v>
       </c>
       <c r="J330" s="4" t="s">
-        <v>1613</v>
+        <v>1324</v>
       </c>
       <c r="K330" s="1" t="s">
         <v>1324</v>
@@ -62280,7 +62285,7 @@
         <v>326</v>
       </c>
       <c r="J331" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K331" s="1" t="s">
         <v>1324</v>
@@ -62309,7 +62314,7 @@
         <v>327</v>
       </c>
       <c r="J332" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K332" s="1" t="s">
         <v>1324</v>
@@ -62338,7 +62343,7 @@
         <v>328</v>
       </c>
       <c r="J333" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K333" s="1" t="s">
         <v>1324</v>
@@ -62367,7 +62372,7 @@
         <v>329</v>
       </c>
       <c r="J334" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K334" s="1" t="s">
         <v>1324</v>
@@ -62396,7 +62401,7 @@
         <v>330</v>
       </c>
       <c r="J335" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K335" s="1" t="s">
         <v>1324</v>
@@ -62425,7 +62430,7 @@
         <v>331</v>
       </c>
       <c r="J336" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K336" s="1" t="s">
         <v>1324</v>
@@ -62454,7 +62459,7 @@
         <v>332</v>
       </c>
       <c r="J337" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K337" s="1" t="s">
         <v>1324</v>
@@ -62483,7 +62488,7 @@
         <v>333</v>
       </c>
       <c r="J338" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K338" s="1" t="s">
         <v>1324</v>
@@ -62512,7 +62517,7 @@
         <v>334</v>
       </c>
       <c r="J339" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K339" s="1" t="s">
         <v>1324</v>
@@ -62541,7 +62546,7 @@
         <v>335</v>
       </c>
       <c r="J340" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K340" s="1" t="s">
         <v>1324</v>
@@ -62570,7 +62575,7 @@
         <v>336</v>
       </c>
       <c r="J341" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K341" s="1" t="s">
         <v>1324</v>
@@ -62599,7 +62604,7 @@
         <v>337</v>
       </c>
       <c r="J342" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K342" s="1" t="s">
         <v>1324</v>
@@ -62628,7 +62633,7 @@
         <v>338</v>
       </c>
       <c r="J343" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K343" s="1" t="s">
         <v>1324</v>
@@ -62657,7 +62662,7 @@
         <v>339</v>
       </c>
       <c r="J344" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K344" s="1" t="s">
         <v>1324</v>
@@ -62686,7 +62691,7 @@
         <v>340</v>
       </c>
       <c r="J345" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K345" s="1" t="s">
         <v>1324</v>
@@ -62718,7 +62723,7 @@
         <v>711</v>
       </c>
       <c r="J346" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K346" s="1" t="s">
         <v>1324</v>
@@ -62747,7 +62752,7 @@
         <v>342</v>
       </c>
       <c r="J347" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K347" s="1" t="s">
         <v>1324</v>
@@ -62776,7 +62781,7 @@
         <v>343</v>
       </c>
       <c r="J348" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K348" s="1" t="s">
         <v>1324</v>
@@ -62805,7 +62810,7 @@
         <v>344</v>
       </c>
       <c r="J349" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K349" s="1" t="s">
         <v>1324</v>
@@ -62834,7 +62839,7 @@
         <v>345</v>
       </c>
       <c r="J350" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K350" s="1" t="s">
         <v>1324</v>
@@ -62863,7 +62868,7 @@
         <v>346</v>
       </c>
       <c r="J351" s="4" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="K351" s="1" t="s">
         <v>1324</v>
@@ -62892,7 +62897,7 @@
         <v>347</v>
       </c>
       <c r="J352" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K352" s="1" t="s">
         <v>1324</v>
@@ -62921,7 +62926,7 @@
         <v>348</v>
       </c>
       <c r="J353" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K353" s="1" t="s">
         <v>1324</v>
@@ -62950,7 +62955,7 @@
         <v>349</v>
       </c>
       <c r="J354" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K354" s="1" t="s">
         <v>1324</v>
@@ -62979,7 +62984,7 @@
         <v>350</v>
       </c>
       <c r="J355" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K355" s="1" t="s">
         <v>1324</v>
@@ -63008,7 +63013,7 @@
         <v>351</v>
       </c>
       <c r="J356" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K356" s="1" t="s">
         <v>1324</v>
@@ -63037,7 +63042,7 @@
         <v>352</v>
       </c>
       <c r="J357" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K357" s="1" t="s">
         <v>1324</v>
@@ -63069,7 +63074,7 @@
         <v>711</v>
       </c>
       <c r="J358" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K358" s="1" t="s">
         <v>1324</v>
@@ -63098,7 +63103,7 @@
         <v>354</v>
       </c>
       <c r="J359" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K359" s="1" t="s">
         <v>1324</v>
@@ -63127,7 +63132,7 @@
         <v>355</v>
       </c>
       <c r="J360" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K360" s="1" t="s">
         <v>1324</v>
@@ -63156,14 +63161,13 @@
         <v>356</v>
       </c>
       <c r="J361" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="K361" s="1" t="s">
         <v>1324</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K361" xr:uid="{C9791905-45CB-4A13-A607-A158D8B6240A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v0.9.1 - Add a cool dynamic subtitle in figure 2 to help with interpretability
</commit_message>
<xml_diff>
--- a/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
+++ b/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpascariu\Documents\R-Repos\lemur\data-raw\GBD_2019_Data_Tools_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F8CA6A-54C7-4576-941F-65049A93AD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABB2704-7C96-408F-9F65-45CD6AADCBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GBD 2019 Locations Hierarchy" sheetId="4" r:id="rId1"/>
@@ -18753,7 +18753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1690"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -57647,9 +57647,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N361"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B334" sqref="B334"/>
+      <selection pane="bottomLeft" activeCell="B366" sqref="B366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57663,7 +57663,7 @@
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="18" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" style="18" customWidth="1"/>
     <col min="11" max="11" width="19" style="19" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="13.140625" customWidth="1"/>
@@ -58241,7 +58241,7 @@
       </c>
       <c r="N17" s="9"/>
     </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>297</v>
       </c>
@@ -58774,7 +58774,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>345</v>
       </c>
@@ -60091,7 +60091,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="74" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>366</v>
       </c>
@@ -60458,7 +60458,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="85" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>380</v>
       </c>
@@ -65189,7 +65189,7 @@
         <v>-33</v>
       </c>
     </row>
-    <row r="229" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>587</v>
       </c>
@@ -68728,7 +68728,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="334" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="3">
         <v>700</v>
       </c>
@@ -69217,7 +69217,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="349" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3">
         <v>729</v>
       </c>
@@ -69325,7 +69325,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="352" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3">
         <v>718</v>
       </c>
@@ -69656,9 +69656,25 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N361" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="11">
+    <filterColumn colId="9">
       <filters>
-        <filter val="yes"/>
+        <filter val="Chronic Respiratory diseases"/>
+        <filter val="Colon and Rectum Cancer"/>
+        <filter val="Diabetes and Kidney Diseases"/>
+        <filter val="Digestive Diseases"/>
+        <filter val="HIV/ AIDS / STD"/>
+        <filter val="Infections (excl. Respiratory)"/>
+        <filter val="Injuries"/>
+        <filter val="Ischemic Heart Disease"/>
+        <filter val="Lung Cancer"/>
+        <filter val="Maternal and Neonatal"/>
+        <filter val="Neurological Disorders"/>
+        <filter val="Other Cardiovascular"/>
+        <filter val="Other Neoplasms"/>
+        <filter val="Other Non-Communicable"/>
+        <filter val="Respiratory Infections"/>
+        <filter val="Self-Harm and Violence"/>
+        <filter val="Stroke"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
v0.11.0 - Add new functionality (boomarks, reset) and provide a more consistet arrangement of the cod with the ICD classification;
</commit_message>
<xml_diff>
--- a/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
+++ b/data-raw/GBD_2019_Data_Tools_Guide/IHME_GBD_2019_A1_HIERARCHIES_Y2020M10D15.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpascariu\Documents\R-Repos\lemur\data-raw\GBD_2019_Data_Tools_Guide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABB2704-7C96-408F-9F65-45CD6AADCBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2BDED9-5265-46C9-B99E-D5272197373C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6706" uniqueCount="1646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6708" uniqueCount="1648">
   <si>
     <t>Global</t>
   </si>
@@ -4976,6 +4976,12 @@
   </si>
   <si>
     <t>Download</t>
+  </si>
+  <si>
+    <t>sdg_order</t>
+  </si>
+  <si>
+    <t>cod_order</t>
   </si>
 </sst>
 </file>
@@ -57645,11 +57651,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N361"/>
+  <dimension ref="A1:P361"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B366" sqref="B366"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57667,9 +57673,10 @@
     <col min="11" max="11" width="19" style="19" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>679</v>
       </c>
@@ -57712,8 +57719,14 @@
       <c r="N1" s="5" t="s">
         <v>1643</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="11" t="s">
+        <v>1647</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>294</v>
       </c>
@@ -57745,7 +57758,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>295</v>
       </c>
@@ -57777,7 +57790,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>955</v>
       </c>
@@ -57814,8 +57827,14 @@
       <c r="N4" s="2">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="2">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>298</v>
       </c>
@@ -57847,7 +57866,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>948</v>
       </c>
@@ -57879,7 +57898,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>949</v>
       </c>
@@ -57911,7 +57930,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>950</v>
       </c>
@@ -57943,7 +57962,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>300</v>
       </c>
@@ -57975,7 +57994,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>393</v>
       </c>
@@ -58007,7 +58026,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>394</v>
       </c>
@@ -58039,7 +58058,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>395</v>
       </c>
@@ -58071,7 +58090,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>396</v>
       </c>
@@ -58103,7 +58122,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>397</v>
       </c>
@@ -58138,7 +58157,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>398</v>
       </c>
@@ -58173,7 +58192,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>399</v>
       </c>
@@ -58205,7 +58224,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>956</v>
       </c>
@@ -58240,8 +58259,14 @@
         <v>1642</v>
       </c>
       <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="2">
+        <v>11</v>
+      </c>
+      <c r="P17" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>297</v>
       </c>
@@ -58278,8 +58303,11 @@
       <c r="N18" s="3">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>954</v>
       </c>
@@ -58314,7 +58342,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>934</v>
       </c>
@@ -58346,7 +58374,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>946</v>
       </c>
@@ -58378,7 +58406,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>947</v>
       </c>
@@ -58410,7 +58438,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>322</v>
       </c>
@@ -58442,7 +58470,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>328</v>
       </c>
@@ -58474,7 +58502,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>329</v>
       </c>
@@ -58506,7 +58534,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>957</v>
       </c>
@@ -58543,8 +58571,14 @@
       <c r="N26" s="20">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>302</v>
       </c>
@@ -58576,7 +58610,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>958</v>
       </c>
@@ -58608,7 +58642,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>319</v>
       </c>
@@ -58640,7 +58674,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>320</v>
       </c>
@@ -58672,7 +58706,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>959</v>
       </c>
@@ -58704,7 +58738,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>321</v>
       </c>
@@ -58736,7 +58770,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>344</v>
       </c>
@@ -58773,8 +58807,14 @@
       <c r="N33" s="2">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O33" s="2">
+        <v>1</v>
+      </c>
+      <c r="P33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>345</v>
       </c>
@@ -58811,8 +58851,11 @@
       <c r="N34" s="3">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>346</v>
       </c>
@@ -58844,7 +58887,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>347</v>
       </c>
@@ -58876,7 +58919,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>348</v>
       </c>
@@ -58908,7 +58951,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>349</v>
       </c>
@@ -58943,7 +58986,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>350</v>
       </c>
@@ -58975,7 +59018,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>351</v>
       </c>
@@ -59007,7 +59050,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>352</v>
       </c>
@@ -59039,7 +59082,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>353</v>
       </c>
@@ -59071,7 +59114,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>354</v>
       </c>
@@ -59106,7 +59149,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>355</v>
       </c>
@@ -59141,7 +59184,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>356</v>
       </c>
@@ -59176,7 +59219,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>357</v>
       </c>
@@ -59208,7 +59251,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>358</v>
       </c>
@@ -59240,7 +59283,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>359</v>
       </c>
@@ -59272,7 +59315,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>360</v>
       </c>
@@ -59304,7 +59347,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>361</v>
       </c>
@@ -59336,7 +59379,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>362</v>
       </c>
@@ -59371,7 +59414,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>363</v>
       </c>
@@ -59406,7 +59449,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="53" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>364</v>
       </c>
@@ -59441,7 +59484,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="54" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>405</v>
       </c>
@@ -59476,7 +59519,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="55" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>843</v>
       </c>
@@ -59508,7 +59551,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>935</v>
       </c>
@@ -59540,7 +59583,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>936</v>
       </c>
@@ -59575,7 +59618,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="58" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>365</v>
       </c>
@@ -59607,7 +59650,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>961</v>
       </c>
@@ -59642,8 +59685,14 @@
         <v>1642</v>
       </c>
       <c r="N59" s="9"/>
-    </row>
-    <row r="60" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O59" s="2">
+        <v>1</v>
+      </c>
+      <c r="P59" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>332</v>
       </c>
@@ -59675,7 +59724,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>337</v>
       </c>
@@ -59707,7 +59756,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="62" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>338</v>
       </c>
@@ -59739,7 +59788,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>339</v>
       </c>
@@ -59771,7 +59820,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>340</v>
       </c>
@@ -59803,7 +59852,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>341</v>
       </c>
@@ -59835,7 +59884,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>342</v>
       </c>
@@ -59867,7 +59916,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="67" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>400</v>
       </c>
@@ -59899,7 +59948,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>401</v>
       </c>
@@ -59931,7 +59980,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>402</v>
       </c>
@@ -59963,7 +60012,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>403</v>
       </c>
@@ -59995,7 +60044,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>404</v>
       </c>
@@ -60027,7 +60076,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="72" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>408</v>
       </c>
@@ -60059,7 +60108,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="73" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>962</v>
       </c>
@@ -60090,8 +60139,11 @@
       <c r="L73" s="6" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O73" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>366</v>
       </c>
@@ -60128,8 +60180,11 @@
       <c r="N74" s="3">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P74" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>367</v>
       </c>
@@ -60161,7 +60216,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>368</v>
       </c>
@@ -60193,7 +60248,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>369</v>
       </c>
@@ -60225,7 +60280,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>370</v>
       </c>
@@ -60257,7 +60312,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>995</v>
       </c>
@@ -60289,7 +60344,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>374</v>
       </c>
@@ -60321,7 +60376,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>375</v>
       </c>
@@ -60356,7 +60411,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>376</v>
       </c>
@@ -60391,7 +60446,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>741</v>
       </c>
@@ -60426,7 +60481,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>379</v>
       </c>
@@ -60458,7 +60513,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="85" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>380</v>
       </c>
@@ -60495,8 +60550,11 @@
       <c r="N85" s="3">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P85" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>381</v>
       </c>
@@ -60528,7 +60586,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>382</v>
       </c>
@@ -60560,7 +60618,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>383</v>
       </c>
@@ -60592,7 +60650,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>384</v>
       </c>
@@ -60624,7 +60682,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>385</v>
       </c>
@@ -60656,7 +60714,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="91" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>386</v>
       </c>
@@ -60692,8 +60750,14 @@
         <v>NA</v>
       </c>
       <c r="N91" s="9"/>
-    </row>
-    <row r="92" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O91" s="2">
+        <v>1</v>
+      </c>
+      <c r="P91" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>387</v>
       </c>
@@ -60725,7 +60789,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="93" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>388</v>
       </c>
@@ -60760,7 +60824,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="94" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>389</v>
       </c>
@@ -60795,7 +60859,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="95" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>390</v>
       </c>
@@ -60830,7 +60894,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="96" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>391</v>
       </c>
@@ -60862,7 +60926,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>409</v>
       </c>
@@ -60894,7 +60958,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="98" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>410</v>
       </c>
@@ -60931,8 +60995,14 @@
       <c r="N98" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O98" s="2">
+        <v>5</v>
+      </c>
+      <c r="P98" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>444</v>
       </c>
@@ -60964,7 +61034,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="100" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>447</v>
       </c>
@@ -60996,7 +61066,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="101" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>450</v>
       </c>
@@ -61028,7 +61098,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="102" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>411</v>
       </c>
@@ -61060,7 +61130,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="103" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>414</v>
       </c>
@@ -61092,7 +61162,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="104" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>441</v>
       </c>
@@ -61123,8 +61193,11 @@
       <c r="L104" s="7" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O104" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>417</v>
       </c>
@@ -61156,7 +61229,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>418</v>
       </c>
@@ -61188,7 +61261,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>419</v>
       </c>
@@ -61220,7 +61293,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>420</v>
       </c>
@@ -61252,7 +61325,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>996</v>
       </c>
@@ -61284,7 +61357,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1021</v>
       </c>
@@ -61316,7 +61389,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="111" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>453</v>
       </c>
@@ -61348,7 +61421,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="112" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>456</v>
       </c>
@@ -61380,7 +61453,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="113" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>423</v>
       </c>
@@ -61412,7 +61485,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="114" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>426</v>
       </c>
@@ -61443,8 +61516,11 @@
       <c r="L114" s="7" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O114" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>459</v>
       </c>
@@ -61476,7 +61552,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="116" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>462</v>
       </c>
@@ -61508,7 +61584,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>849</v>
       </c>
@@ -61540,7 +61616,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>850</v>
       </c>
@@ -61575,7 +61651,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>429</v>
       </c>
@@ -61607,7 +61683,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="120" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>432</v>
       </c>
@@ -61639,7 +61715,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="121" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>435</v>
       </c>
@@ -61671,7 +61747,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="122" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>465</v>
       </c>
@@ -61703,7 +61779,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="123" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>438</v>
       </c>
@@ -61735,7 +61811,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="124" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>468</v>
       </c>
@@ -61767,7 +61843,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="125" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>471</v>
       </c>
@@ -61799,7 +61875,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="126" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>474</v>
       </c>
@@ -61831,7 +61907,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="127" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>477</v>
       </c>
@@ -61863,7 +61939,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="128" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>480</v>
       </c>
@@ -62416,7 +62492,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="145" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>491</v>
       </c>
@@ -62453,8 +62529,14 @@
       <c r="N145" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O145" s="2">
+        <v>10</v>
+      </c>
+      <c r="P145" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>492</v>
       </c>
@@ -62486,7 +62568,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="147" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>493</v>
       </c>
@@ -62517,8 +62599,11 @@
       <c r="L147" s="7" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O147" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>494</v>
       </c>
@@ -62549,8 +62634,11 @@
       <c r="L148" s="7" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O148" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>495</v>
       </c>
@@ -62582,7 +62670,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>496</v>
       </c>
@@ -62614,7 +62702,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>497</v>
       </c>
@@ -62646,7 +62734,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="152" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>498</v>
       </c>
@@ -62678,7 +62766,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="153" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>504</v>
       </c>
@@ -62710,7 +62798,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>968</v>
       </c>
@@ -62742,7 +62830,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>969</v>
       </c>
@@ -62774,7 +62862,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>970</v>
       </c>
@@ -62806,7 +62894,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="157" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>499</v>
       </c>
@@ -62838,7 +62926,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>942</v>
       </c>
@@ -62870,7 +62958,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>938</v>
       </c>
@@ -62902,7 +62990,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>944</v>
       </c>
@@ -62934,7 +63022,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="161" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>500</v>
       </c>
@@ -62966,7 +63054,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="162" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>501</v>
       </c>
@@ -63001,7 +63089,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="163" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>502</v>
       </c>
@@ -63033,7 +63121,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="164" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>503</v>
       </c>
@@ -63065,7 +63153,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="165" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>1023</v>
       </c>
@@ -63097,7 +63185,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="166" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>508</v>
       </c>
@@ -63134,8 +63222,14 @@
       <c r="N166" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O166" s="2">
+        <v>12</v>
+      </c>
+      <c r="P166" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>509</v>
       </c>
@@ -63167,7 +63261,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="168" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>510</v>
       </c>
@@ -63199,7 +63293,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>511</v>
       </c>
@@ -63231,7 +63325,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>512</v>
       </c>
@@ -63263,7 +63357,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>513</v>
       </c>
@@ -63295,7 +63389,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>514</v>
       </c>
@@ -63327,7 +63421,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="173" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>515</v>
       </c>
@@ -63359,7 +63453,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="174" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>516</v>
       </c>
@@ -63391,7 +63485,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="175" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>520</v>
       </c>
@@ -63423,7 +63517,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="176" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>526</v>
       </c>
@@ -63458,6 +63552,12 @@
         <v>1642</v>
       </c>
       <c r="N176" s="9"/>
+      <c r="O176" s="2">
+        <v>13</v>
+      </c>
+      <c r="P176" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="177" spans="1:12" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
@@ -63974,7 +64074,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="193" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>535</v>
       </c>
@@ -64006,7 +64106,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="194" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>541</v>
       </c>
@@ -64038,7 +64138,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="195" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>542</v>
       </c>
@@ -64074,8 +64174,14 @@
         <v>NA</v>
       </c>
       <c r="N195" s="9"/>
-    </row>
-    <row r="196" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O195" s="2">
+        <v>7</v>
+      </c>
+      <c r="P195" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>543</v>
       </c>
@@ -64107,7 +64213,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="197" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>544</v>
       </c>
@@ -64139,7 +64245,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="198" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>545</v>
       </c>
@@ -64171,7 +64277,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="199" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>546</v>
       </c>
@@ -64203,7 +64309,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="200" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>554</v>
       </c>
@@ -64235,7 +64341,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="201" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>972</v>
       </c>
@@ -64270,7 +64376,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>547</v>
       </c>
@@ -64305,7 +64411,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>548</v>
       </c>
@@ -64340,7 +64446,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="204" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>557</v>
       </c>
@@ -64372,7 +64478,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="205" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>558</v>
       </c>
@@ -64408,8 +64514,14 @@
         <v>NA</v>
       </c>
       <c r="N205" s="9"/>
-    </row>
-    <row r="206" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O205" s="2">
+        <v>15</v>
+      </c>
+      <c r="P205" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>559</v>
       </c>
@@ -64444,7 +64556,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="207" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>567</v>
       </c>
@@ -64479,7 +64591,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>568</v>
       </c>
@@ -64514,7 +64626,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>569</v>
       </c>
@@ -64549,7 +64661,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="210" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>570</v>
       </c>
@@ -64584,7 +64696,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="211" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>571</v>
       </c>
@@ -64619,7 +64731,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="212" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>572</v>
       </c>
@@ -64651,7 +64763,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>573</v>
       </c>
@@ -64683,7 +64795,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>574</v>
       </c>
@@ -64715,7 +64827,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="215" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>575</v>
       </c>
@@ -64750,7 +64862,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="216" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>578</v>
       </c>
@@ -64785,7 +64897,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="217" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>579</v>
       </c>
@@ -64820,7 +64932,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="218" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>582</v>
       </c>
@@ -64855,7 +64967,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="219" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>585</v>
       </c>
@@ -64890,7 +65002,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="220" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>973</v>
       </c>
@@ -64926,8 +65038,14 @@
         <v>NA</v>
       </c>
       <c r="N220" s="9"/>
-    </row>
-    <row r="221" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O220" s="2">
+        <v>15</v>
+      </c>
+      <c r="P220" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>560</v>
       </c>
@@ -64959,7 +65077,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="222" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>561</v>
       </c>
@@ -64991,7 +65109,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>562</v>
       </c>
@@ -65023,7 +65141,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>563</v>
       </c>
@@ -65055,7 +65173,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>564</v>
       </c>
@@ -65087,7 +65205,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>565</v>
       </c>
@@ -65122,7 +65240,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>566</v>
       </c>
@@ -65154,7 +65272,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="228" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>974</v>
       </c>
@@ -65188,8 +65306,14 @@
       <c r="M228" s="2">
         <v>-33</v>
       </c>
-    </row>
-    <row r="229" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O228" s="2">
+        <v>6</v>
+      </c>
+      <c r="P228" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>587</v>
       </c>
@@ -65226,8 +65350,11 @@
       <c r="N229" s="3">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P229" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>975</v>
       </c>
@@ -65259,7 +65386,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>976</v>
       </c>
@@ -65291,7 +65418,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="232" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>589</v>
       </c>
@@ -65323,7 +65450,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>997</v>
       </c>
@@ -65355,7 +65482,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>998</v>
       </c>
@@ -65387,7 +65514,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>591</v>
       </c>
@@ -65419,7 +65546,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>592</v>
       </c>
@@ -65451,7 +65578,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>593</v>
       </c>
@@ -65483,7 +65610,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="238" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>588</v>
       </c>
@@ -65515,7 +65642,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="239" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>653</v>
       </c>
@@ -65551,8 +65678,14 @@
         <v>NA</v>
       </c>
       <c r="N239" s="9"/>
-    </row>
-    <row r="240" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O239" s="2">
+        <v>15</v>
+      </c>
+      <c r="P239" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>654</v>
       </c>
@@ -66132,7 +66265,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="257" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>669</v>
       </c>
@@ -66171,8 +66304,14 @@
         <v>NA</v>
       </c>
       <c r="N257" s="9"/>
-    </row>
-    <row r="258" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O257" s="2">
+        <v>15</v>
+      </c>
+      <c r="P257" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="3">
         <v>981</v>
       </c>
@@ -66207,7 +66346,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="259" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>670</v>
       </c>
@@ -66242,7 +66381,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="260" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>671</v>
       </c>
@@ -66277,7 +66416,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="261" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>672</v>
       </c>
@@ -66312,7 +66451,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="262" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>999</v>
       </c>
@@ -66347,7 +66486,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="263" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1000</v>
       </c>
@@ -66382,7 +66521,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="264" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>675</v>
       </c>
@@ -66417,7 +66556,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="265" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="3">
         <v>674</v>
       </c>
@@ -66452,7 +66591,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="266" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="3">
         <v>679</v>
       </c>
@@ -66487,7 +66626,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="267" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>626</v>
       </c>
@@ -66523,8 +66662,14 @@
         <v>NA</v>
       </c>
       <c r="N267" s="9"/>
-    </row>
-    <row r="268" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O267" s="2">
+        <v>15</v>
+      </c>
+      <c r="P267" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="268" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="3">
         <v>627</v>
       </c>
@@ -66556,7 +66701,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="269" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="3">
         <v>628</v>
       </c>
@@ -66591,7 +66736,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="270" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1014</v>
       </c>
@@ -66626,7 +66771,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="271" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>1015</v>
       </c>
@@ -66661,7 +66806,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="272" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1016</v>
       </c>
@@ -66696,7 +66841,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="273" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1017</v>
       </c>
@@ -66731,7 +66876,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="274" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="3">
         <v>630</v>
       </c>
@@ -66766,7 +66911,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="275" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3">
         <v>631</v>
       </c>
@@ -66801,7 +66946,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="276" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="3">
         <v>632</v>
       </c>
@@ -66836,7 +66981,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="277" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="3">
         <v>639</v>
       </c>
@@ -66868,7 +67013,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="278" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>640</v>
       </c>
@@ -66904,8 +67049,14 @@
         <v>NA</v>
       </c>
       <c r="N278" s="9"/>
-    </row>
-    <row r="279" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O278" s="2">
+        <v>15</v>
+      </c>
+      <c r="P278" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="3">
         <v>641</v>
       </c>
@@ -66937,7 +67088,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="280" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>642</v>
       </c>
@@ -66969,7 +67120,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="281" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>643</v>
       </c>
@@ -67001,7 +67152,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="282" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>644</v>
       </c>
@@ -67033,7 +67184,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="283" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>645</v>
       </c>
@@ -67065,7 +67216,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="284" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>646</v>
       </c>
@@ -67100,7 +67251,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="285" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>647</v>
       </c>
@@ -67135,7 +67286,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="286" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>648</v>
       </c>
@@ -67167,7 +67318,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="287" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>649</v>
       </c>
@@ -67199,7 +67350,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="288" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>650</v>
       </c>
@@ -68300,7 +68451,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="321" spans="1:14" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>687</v>
       </c>
@@ -68332,7 +68483,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="322" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <v>688</v>
       </c>
@@ -68369,8 +68520,14 @@
       <c r="N322" s="20">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="323" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O322" s="2">
+        <v>16</v>
+      </c>
+      <c r="P322" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="323" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3">
         <v>689</v>
       </c>
@@ -68402,7 +68559,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="324" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>690</v>
       </c>
@@ -68434,7 +68591,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>691</v>
       </c>
@@ -68466,7 +68623,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>692</v>
       </c>
@@ -68498,7 +68655,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="327" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>693</v>
       </c>
@@ -68530,7 +68687,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>694</v>
       </c>
@@ -68562,7 +68719,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="329" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="3">
         <v>695</v>
       </c>
@@ -68594,7 +68751,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="330" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <v>696</v>
       </c>
@@ -68631,8 +68788,14 @@
       <c r="N330" s="20">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="331" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O330" s="2">
+        <v>16</v>
+      </c>
+      <c r="P330" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="3">
         <v>697</v>
       </c>
@@ -68664,7 +68827,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="332" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="3">
         <v>698</v>
       </c>
@@ -68696,7 +68859,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="333" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="3">
         <v>699</v>
       </c>
@@ -68728,7 +68891,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="334" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A334" s="3">
         <v>700</v>
       </c>
@@ -68765,8 +68928,11 @@
       <c r="N334" s="21">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="335" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P334" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="335" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>701</v>
       </c>
@@ -68798,7 +68964,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="336" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>703</v>
       </c>
@@ -68830,7 +68996,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="337" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="3">
         <v>704</v>
       </c>
@@ -68862,7 +69028,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="338" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>705</v>
       </c>
@@ -68894,7 +69060,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="339" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>707</v>
       </c>
@@ -68926,7 +69092,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="340" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="3">
         <v>708</v>
       </c>
@@ -68958,7 +69124,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="341" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3">
         <v>709</v>
       </c>
@@ -68990,7 +69156,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="342" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>710</v>
       </c>
@@ -69022,7 +69188,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="343" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>711</v>
       </c>
@@ -69054,7 +69220,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="344" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="3">
         <v>712</v>
       </c>
@@ -69086,7 +69252,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="345" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>713</v>
       </c>
@@ -69118,7 +69284,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="346" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>714</v>
       </c>
@@ -69153,7 +69319,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="347" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>715</v>
       </c>
@@ -69185,7 +69351,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="348" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="3">
         <v>842</v>
       </c>
@@ -69217,7 +69383,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="349" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A349" s="3">
         <v>729</v>
       </c>
@@ -69254,8 +69420,11 @@
       <c r="N349" s="21" t="s">
         <v>1644</v>
       </c>
-    </row>
-    <row r="350" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P349" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="350" spans="1:16" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3">
         <v>716</v>
       </c>
@@ -69287,7 +69456,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="351" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <v>717</v>
       </c>
@@ -69324,8 +69493,14 @@
       <c r="N351" s="20">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="352" spans="1:14" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O351" s="2">
+        <v>17</v>
+      </c>
+      <c r="P351" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="352" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A352" s="3">
         <v>718</v>
       </c>
@@ -69361,6 +69536,9 @@
       </c>
       <c r="N352" s="21">
         <v>3.4</v>
+      </c>
+      <c r="P352" s="3">
+        <v>21</v>
       </c>
     </row>
     <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
@@ -69656,25 +69834,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N361" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="9">
+    <filterColumn colId="11">
       <filters>
-        <filter val="Chronic Respiratory diseases"/>
-        <filter val="Colon and Rectum Cancer"/>
-        <filter val="Diabetes and Kidney Diseases"/>
-        <filter val="Digestive Diseases"/>
-        <filter val="HIV/ AIDS / STD"/>
-        <filter val="Infections (excl. Respiratory)"/>
-        <filter val="Injuries"/>
-        <filter val="Ischemic Heart Disease"/>
-        <filter val="Lung Cancer"/>
-        <filter val="Maternal and Neonatal"/>
-        <filter val="Neurological Disorders"/>
-        <filter val="Other Cardiovascular"/>
-        <filter val="Other Neoplasms"/>
-        <filter val="Other Non-Communicable"/>
-        <filter val="Respiratory Infections"/>
-        <filter val="Self-Harm and Violence"/>
-        <filter val="Stroke"/>
+        <filter val="yes"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>